<commit_message>
trace of tahara at bendol bhitri baato
</commit_message>
<xml_diff>
--- a/ofc/estimates/परोपकार भवन मर्मत/V-परोपकार भवन मर्मत.xlsx
+++ b/ofc/estimates/परोपकार भवन मर्मत/V-परोपकार भवन मर्मत.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\परोपकार भवन मर्मत\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\परोपकार भवन मर्मत\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="backyard" sheetId="22" r:id="rId1"/>
@@ -116,7 +116,7 @@
     <definedName name="Ttile">'[1]update Rate'!$N$43</definedName>
     <definedName name="unskilled">'[2]Material rate'!$D$154</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="167">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -864,15 +864,21 @@
   <si>
     <t>at compound</t>
   </si>
+  <si>
+    <t>Detail Valuated Sheet</t>
+  </si>
+  <si>
+    <t>Total Valuated</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="50">
     <font>
@@ -1265,10 +1271,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="222">
+  <cellXfs count="223">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1276,7 +1282,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1296,14 +1302,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1312,7 +1318,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1336,7 +1342,7 @@
     <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1371,7 +1377,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1386,7 +1392,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1402,7 +1408,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1444,7 +1450,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
@@ -1482,7 +1488,7 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1569,7 +1575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1593,7 +1599,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1617,115 +1623,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="41" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1735,7 +1632,7 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="42" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="42" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1784,7 +1681,7 @@
     <xf numFmtId="0" fontId="43" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="42" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="42" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="41" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1812,6 +1709,118 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2810,127 +2819,127 @@
       <selection activeCell="A104" sqref="A104:XFD104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="188" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-      <c r="J1" s="159"/>
-      <c r="K1" s="159"/>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8">
-      <c r="A2" s="160" t="s">
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
+      <c r="K1" s="188"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5">
+      <c r="A2" s="189" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
-      <c r="J2" s="160"/>
-      <c r="K2" s="160"/>
+      <c r="B2" s="189"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="189"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="189"/>
+      <c r="H2" s="189"/>
+      <c r="I2" s="189"/>
+      <c r="J2" s="189"/>
+      <c r="K2" s="189"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="148"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="148"/>
-      <c r="G3" s="148"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="148"/>
+      <c r="B3" s="190"/>
+      <c r="C3" s="190"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="190"/>
+      <c r="F3" s="190"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="190"/>
+      <c r="J3" s="190"/>
+      <c r="K3" s="190"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="148" t="s">
+      <c r="A4" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="148"/>
-      <c r="C4" s="148"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="148"/>
-      <c r="G4" s="148"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
-      <c r="K4" s="148"/>
-    </row>
-    <row r="5" spans="1:14" ht="17.399999999999999">
-      <c r="A5" s="161" t="s">
+      <c r="B4" s="190"/>
+      <c r="C4" s="190"/>
+      <c r="D4" s="190"/>
+      <c r="E4" s="190"/>
+      <c r="F4" s="190"/>
+      <c r="G4" s="190"/>
+      <c r="H4" s="190"/>
+      <c r="I4" s="190"/>
+      <c r="J4" s="190"/>
+      <c r="K4" s="190"/>
+    </row>
+    <row r="5" spans="1:14" ht="18.75">
+      <c r="A5" s="191" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="161"/>
-      <c r="C5" s="161"/>
-      <c r="D5" s="161"/>
-      <c r="E5" s="161"/>
-      <c r="F5" s="161"/>
-      <c r="G5" s="161"/>
-      <c r="H5" s="161"/>
-      <c r="I5" s="161"/>
-      <c r="J5" s="161"/>
-      <c r="K5" s="161"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.6">
-      <c r="A6" s="152" t="s">
+      <c r="B5" s="191"/>
+      <c r="C5" s="191"/>
+      <c r="D5" s="191"/>
+      <c r="E5" s="191"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="191"/>
+      <c r="I5" s="191"/>
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75">
+      <c r="A6" s="192" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="152"/>
-      <c r="C6" s="152"/>
-      <c r="D6" s="152"/>
-      <c r="E6" s="152"/>
-      <c r="F6" s="152"/>
+      <c r="B6" s="192"/>
+      <c r="C6" s="192"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="192"/>
+      <c r="F6" s="192"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="158" t="s">
+      <c r="H6" s="193" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="158"/>
-      <c r="J6" s="158"/>
-      <c r="K6" s="158"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.6">
-      <c r="A7" s="162" t="s">
+      <c r="I6" s="193"/>
+      <c r="J6" s="193"/>
+      <c r="K6" s="193"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75">
+      <c r="A7" s="194" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="162"/>
-      <c r="C7" s="162"/>
-      <c r="D7" s="162"/>
-      <c r="E7" s="162"/>
-      <c r="F7" s="162"/>
+      <c r="B7" s="194"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="163" t="s">
+      <c r="H7" s="195" t="s">
         <v>158</v>
       </c>
-      <c r="I7" s="163"/>
-      <c r="J7" s="163"/>
-      <c r="K7" s="163"/>
+      <c r="I7" s="195"/>
+      <c r="J7" s="195"/>
+      <c r="K7" s="195"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -2967,7 +2976,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="27.6">
+    <row r="9" spans="1:14" ht="28.5">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -3055,7 +3064,7 @@
       <c r="J12" s="40"/>
       <c r="K12" s="21"/>
     </row>
-    <row r="13" spans="1:14" ht="27.6">
+    <row r="13" spans="1:14" ht="28.5">
       <c r="A13" s="18">
         <v>2</v>
       </c>
@@ -3186,7 +3195,7 @@
       <c r="J18" s="40"/>
       <c r="K18" s="21"/>
     </row>
-    <row r="19" spans="1:14" s="1" customFormat="1" ht="55.2">
+    <row r="19" spans="1:14" s="1" customFormat="1" ht="57">
       <c r="A19" s="58">
         <v>3</v>
       </c>
@@ -3341,7 +3350,7 @@
       <c r="J25" s="40"/>
       <c r="K25" s="21"/>
     </row>
-    <row r="26" spans="1:14" ht="27.6">
+    <row r="26" spans="1:14" ht="28.5">
       <c r="A26" s="18">
         <v>4</v>
       </c>
@@ -3444,7 +3453,7 @@
       <c r="J30" s="40"/>
       <c r="K30" s="21"/>
     </row>
-    <row r="31" spans="1:14" ht="27.6">
+    <row r="31" spans="1:14" ht="28.5">
       <c r="A31" s="18">
         <v>5</v>
       </c>
@@ -3544,7 +3553,7 @@
       <c r="J35" s="40"/>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:19" ht="41.4">
+    <row r="36" spans="1:19" ht="42.75">
       <c r="A36" s="18">
         <v>6</v>
       </c>
@@ -3648,7 +3657,7 @@
       <c r="J40" s="40"/>
       <c r="K40" s="21"/>
     </row>
-    <row r="41" spans="1:19" ht="30.6">
+    <row r="41" spans="1:19" ht="30.75">
       <c r="A41" s="18">
         <v>7</v>
       </c>
@@ -3737,7 +3746,7 @@
       <c r="J44" s="39"/>
       <c r="K44" s="21"/>
     </row>
-    <row r="45" spans="1:19" ht="15">
+    <row r="45" spans="1:19">
       <c r="A45" s="18">
         <v>8</v>
       </c>
@@ -4042,7 +4051,7 @@
       </c>
       <c r="K57" s="21"/>
     </row>
-    <row r="58" spans="1:20" ht="15">
+    <row r="58" spans="1:20">
       <c r="A58" s="18"/>
       <c r="B58" s="88"/>
       <c r="C58" s="19"/>
@@ -4055,7 +4064,7 @@
       <c r="J58" s="39"/>
       <c r="K58" s="21"/>
     </row>
-    <row r="59" spans="1:20" ht="39">
+    <row r="59" spans="1:20" ht="39.75">
       <c r="A59" s="18">
         <v>10</v>
       </c>
@@ -4107,15 +4116,15 @@
       <c r="I60" s="38"/>
       <c r="J60" s="38"/>
       <c r="K60" s="60"/>
-      <c r="N60" s="166" t="s">
+      <c r="N60" s="196" t="s">
         <v>87</v>
       </c>
-      <c r="O60" s="166"/>
-      <c r="P60" s="166"/>
-      <c r="Q60" s="166"/>
-      <c r="R60" s="166"/>
-      <c r="S60" s="166"/>
-      <c r="T60" s="166"/>
+      <c r="O60" s="196"/>
+      <c r="P60" s="196"/>
+      <c r="Q60" s="196"/>
+      <c r="R60" s="196"/>
+      <c r="S60" s="196"/>
+      <c r="T60" s="196"/>
     </row>
     <row r="61" spans="1:20" ht="15" customHeight="1">
       <c r="A61" s="18"/>
@@ -4412,15 +4421,15 @@
       <c r="I73" s="38"/>
       <c r="J73" s="38"/>
       <c r="K73" s="60"/>
-      <c r="N73" s="166" t="s">
+      <c r="N73" s="196" t="s">
         <v>87</v>
       </c>
-      <c r="O73" s="166"/>
-      <c r="P73" s="166"/>
-      <c r="Q73" s="166"/>
-      <c r="R73" s="166"/>
-      <c r="S73" s="166"/>
-      <c r="T73" s="166"/>
+      <c r="O73" s="196"/>
+      <c r="P73" s="196"/>
+      <c r="Q73" s="196"/>
+      <c r="R73" s="196"/>
+      <c r="S73" s="196"/>
+      <c r="T73" s="196"/>
     </row>
     <row r="74" spans="1:20" ht="15" customHeight="1">
       <c r="A74" s="18"/>
@@ -4616,15 +4625,15 @@
       <c r="I81" s="38"/>
       <c r="J81" s="38"/>
       <c r="K81" s="60"/>
-      <c r="N81" s="166" t="s">
+      <c r="N81" s="196" t="s">
         <v>87</v>
       </c>
-      <c r="O81" s="166"/>
-      <c r="P81" s="166"/>
-      <c r="Q81" s="166"/>
-      <c r="R81" s="166"/>
-      <c r="S81" s="166"/>
-      <c r="T81" s="166"/>
+      <c r="O81" s="196"/>
+      <c r="P81" s="196"/>
+      <c r="Q81" s="196"/>
+      <c r="R81" s="196"/>
+      <c r="S81" s="196"/>
+      <c r="T81" s="196"/>
     </row>
     <row r="82" spans="1:20" ht="15" customHeight="1">
       <c r="A82" s="18"/>
@@ -4747,7 +4756,7 @@
       <c r="J86" s="40"/>
       <c r="K86" s="21"/>
     </row>
-    <row r="87" spans="1:20" ht="30.6">
+    <row r="87" spans="1:20" ht="30.75">
       <c r="A87" s="18">
         <v>14</v>
       </c>
@@ -4857,7 +4866,7 @@
       <c r="J90" s="123"/>
       <c r="K90" s="121"/>
     </row>
-    <row r="91" spans="1:20" s="1" customFormat="1" ht="27.6">
+    <row r="91" spans="1:20" s="1" customFormat="1" ht="30">
       <c r="A91" s="120"/>
       <c r="B91" s="125" t="s">
         <v>125</v>
@@ -4915,7 +4924,7 @@
       <c r="K92" s="121"/>
       <c r="M92" s="127"/>
     </row>
-    <row r="93" spans="1:20" s="1" customFormat="1" ht="41.4">
+    <row r="93" spans="1:20" s="1" customFormat="1" ht="45">
       <c r="A93" s="120"/>
       <c r="B93" s="125" t="s">
         <v>126</v>
@@ -5027,7 +5036,7 @@
       <c r="K96" s="121"/>
       <c r="M96" s="127"/>
     </row>
-    <row r="97" spans="1:13" s="1" customFormat="1" ht="27.6">
+    <row r="97" spans="1:13" s="1" customFormat="1" ht="30">
       <c r="A97" s="120"/>
       <c r="B97" s="125" t="s">
         <v>132</v>
@@ -5511,7 +5520,7 @@
       <c r="J117" s="123"/>
       <c r="K117" s="21"/>
     </row>
-    <row r="118" spans="1:11" ht="30.6">
+    <row r="118" spans="1:11" ht="30.75">
       <c r="A118" s="18">
         <v>16</v>
       </c>
@@ -5604,7 +5613,7 @@
       <c r="J122" s="39"/>
       <c r="K122" s="21"/>
     </row>
-    <row r="123" spans="1:11" s="1" customFormat="1" ht="46.2">
+    <row r="123" spans="1:11" s="1" customFormat="1" ht="48">
       <c r="A123" s="18">
         <v>17</v>
       </c>
@@ -5727,7 +5736,7 @@
       <c r="J128" s="39"/>
       <c r="K128" s="21"/>
     </row>
-    <row r="129" spans="1:20" s="138" customFormat="1" ht="17.399999999999999">
+    <row r="129" spans="1:20" s="138" customFormat="1" ht="18">
       <c r="A129" s="135">
         <v>18</v>
       </c>
@@ -5852,15 +5861,15 @@
       <c r="J133" s="38"/>
       <c r="K133" s="21"/>
       <c r="M133" s="1"/>
-      <c r="N133" s="180" t="s">
+      <c r="N133" s="186" t="s">
         <v>143</v>
       </c>
-      <c r="O133" s="180"/>
-      <c r="P133" s="180"/>
-      <c r="Q133" s="180"/>
-      <c r="R133" s="180"/>
-      <c r="S133" s="180"/>
-      <c r="T133" s="180"/>
+      <c r="O133" s="186"/>
+      <c r="P133" s="186"/>
+      <c r="Q133" s="186"/>
+      <c r="R133" s="186"/>
+      <c r="S133" s="186"/>
+      <c r="T133" s="186"/>
     </row>
     <row r="134" spans="1:20" ht="15" customHeight="1">
       <c r="A134" s="18"/>
@@ -5885,15 +5894,15 @@
       <c r="J134" s="38"/>
       <c r="K134" s="21"/>
       <c r="M134" s="1"/>
-      <c r="N134" s="180" t="s">
+      <c r="N134" s="186" t="s">
         <v>144</v>
       </c>
-      <c r="O134" s="180"/>
-      <c r="P134" s="180"/>
-      <c r="Q134" s="180"/>
-      <c r="R134" s="180"/>
-      <c r="S134" s="180"/>
-      <c r="T134" s="180"/>
+      <c r="O134" s="186"/>
+      <c r="P134" s="186"/>
+      <c r="Q134" s="186"/>
+      <c r="R134" s="186"/>
+      <c r="S134" s="186"/>
+      <c r="T134" s="186"/>
     </row>
     <row r="135" spans="1:20" ht="15" customHeight="1">
       <c r="A135" s="38"/>
@@ -5952,7 +5961,7 @@
       <c r="J137" s="40"/>
       <c r="K137" s="34"/>
     </row>
-    <row r="138" spans="1:20" ht="41.4">
+    <row r="138" spans="1:20" ht="42.75">
       <c r="A138" s="18">
         <v>19</v>
       </c>
@@ -6172,11 +6181,11 @@
       <c r="B149" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C149" s="164">
+      <c r="C149" s="185">
         <f>J147</f>
         <v>564973.01951057301</v>
       </c>
-      <c r="D149" s="164"/>
+      <c r="D149" s="185"/>
       <c r="E149" s="37">
         <v>100</v>
       </c>
@@ -6192,10 +6201,10 @@
       <c r="B150" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C150" s="165">
+      <c r="C150" s="187">
         <v>500000</v>
       </c>
-      <c r="D150" s="165"/>
+      <c r="D150" s="187"/>
       <c r="E150" s="37"/>
       <c r="F150" s="44"/>
       <c r="G150" s="43"/>
@@ -6209,11 +6218,11 @@
       <c r="B151" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C151" s="165">
+      <c r="C151" s="187">
         <f>C150-C153-C154</f>
         <v>475000</v>
       </c>
-      <c r="D151" s="165"/>
+      <c r="D151" s="187"/>
       <c r="E151" s="37">
         <f>C151/C149*100</f>
         <v>84.074811291251535</v>
@@ -6230,11 +6239,11 @@
       <c r="B152" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C152" s="164">
+      <c r="C152" s="185">
         <f>C149-C151</f>
         <v>89973.019510573009</v>
       </c>
-      <c r="D152" s="164"/>
+      <c r="D152" s="185"/>
       <c r="E152" s="37">
         <f>100-E151</f>
         <v>15.925188708748465</v>
@@ -6251,11 +6260,11 @@
       <c r="B153" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C153" s="164">
+      <c r="C153" s="185">
         <f>C150*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D153" s="164"/>
+      <c r="D153" s="185"/>
       <c r="E153" s="37">
         <v>3</v>
       </c>
@@ -6271,11 +6280,11 @@
       <c r="B154" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C154" s="164">
+      <c r="C154" s="185">
         <f>C150*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D154" s="164"/>
+      <c r="D154" s="185"/>
       <c r="E154" s="37">
         <v>2</v>
       </c>
@@ -6357,13 +6366,6 @@
     <row r="211" s="33" customFormat="1"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C154:D154"/>
-    <mergeCell ref="N134:T134"/>
-    <mergeCell ref="C149:D149"/>
-    <mergeCell ref="C150:D150"/>
-    <mergeCell ref="C151:D151"/>
-    <mergeCell ref="C152:D152"/>
-    <mergeCell ref="C153:D153"/>
     <mergeCell ref="N133:T133"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
@@ -6377,6 +6379,13 @@
     <mergeCell ref="N60:T60"/>
     <mergeCell ref="N73:T73"/>
     <mergeCell ref="N81:T81"/>
+    <mergeCell ref="C154:D154"/>
+    <mergeCell ref="N134:T134"/>
+    <mergeCell ref="C149:D149"/>
+    <mergeCell ref="C150:D150"/>
+    <mergeCell ref="C151:D151"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="C153:D153"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B103" r:id="rId1"/>
@@ -6396,110 +6405,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+    <sheetView topLeftCell="A47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="146" t="s">
+      <c r="A1" s="206" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
-      <c r="J1" s="146"/>
-      <c r="K1" s="146"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6">
-      <c r="A2" s="147" t="s">
+      <c r="B1" s="206"/>
+      <c r="C1" s="206"/>
+      <c r="D1" s="206"/>
+      <c r="E1" s="206"/>
+      <c r="F1" s="206"/>
+      <c r="G1" s="206"/>
+      <c r="H1" s="206"/>
+      <c r="I1" s="206"/>
+      <c r="J1" s="206"/>
+      <c r="K1" s="206"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5">
+      <c r="A2" s="207" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
+      <c r="B2" s="207"/>
+      <c r="C2" s="207"/>
+      <c r="D2" s="207"/>
+      <c r="E2" s="207"/>
+      <c r="F2" s="207"/>
+      <c r="G2" s="207"/>
+      <c r="H2" s="207"/>
+      <c r="I2" s="207"/>
+      <c r="J2" s="207"/>
+      <c r="K2" s="207"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="148"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="148"/>
-      <c r="G3" s="148"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="148"/>
+      <c r="B3" s="190"/>
+      <c r="C3" s="190"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="190"/>
+      <c r="F3" s="190"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="190"/>
+      <c r="J3" s="190"/>
+      <c r="K3" s="190"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1">
-      <c r="A4" s="148" t="s">
+      <c r="A4" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="148"/>
-      <c r="C4" s="148"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="148"/>
-      <c r="G4" s="148"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
-      <c r="K4" s="148"/>
-    </row>
-    <row r="5" spans="1:11" ht="18">
-      <c r="A5" s="149" t="s">
+      <c r="B4" s="190"/>
+      <c r="C4" s="190"/>
+      <c r="D4" s="190"/>
+      <c r="E4" s="190"/>
+      <c r="F4" s="190"/>
+      <c r="G4" s="190"/>
+      <c r="H4" s="190"/>
+      <c r="I4" s="190"/>
+      <c r="J4" s="190"/>
+      <c r="K4" s="190"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75">
+      <c r="A5" s="208" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="149"/>
-      <c r="C5" s="149"/>
-      <c r="D5" s="149"/>
-      <c r="E5" s="149"/>
-      <c r="F5" s="149"/>
-      <c r="G5" s="149"/>
-      <c r="H5" s="149"/>
-      <c r="I5" s="149"/>
-      <c r="J5" s="149"/>
-      <c r="K5" s="149"/>
-    </row>
-    <row r="6" spans="1:11" ht="18">
+      <c r="B5" s="208"/>
+      <c r="C5" s="208"/>
+      <c r="D5" s="208"/>
+      <c r="E5" s="208"/>
+      <c r="F5" s="208"/>
+      <c r="G5" s="208"/>
+      <c r="H5" s="208"/>
+      <c r="I5" s="208"/>
+      <c r="J5" s="208"/>
+      <c r="K5" s="208"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="144">
+      <c r="C6" s="204">
         <f>F71</f>
         <v>564973.01951057301</v>
       </c>
-      <c r="D6" s="145"/>
+      <c r="D6" s="205"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -6507,11 +6516,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="144">
+      <c r="J6" s="204">
         <f>I71</f>
-        <v>450558.50226700824</v>
-      </c>
-      <c r="K6" s="145"/>
+        <v>425480.08486204845</v>
+      </c>
+      <c r="K6" s="205"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="25" t="s">
@@ -6520,77 +6529,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="I7" s="154" t="s">
+      <c r="F7" s="199"/>
+      <c r="G7" s="199"/>
+      <c r="I7" s="200" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="154"/>
-      <c r="K7" s="154"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6">
-      <c r="A8" s="152" t="e">
+      <c r="J7" s="200"/>
+      <c r="K7" s="200"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75">
+      <c r="A8" s="192" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="152"/>
-      <c r="C8" s="152"/>
-      <c r="D8" s="152"/>
-      <c r="E8" s="152"/>
-      <c r="F8" s="152"/>
-      <c r="I8" s="155" t="s">
+      <c r="B8" s="192"/>
+      <c r="C8" s="192"/>
+      <c r="D8" s="192"/>
+      <c r="E8" s="192"/>
+      <c r="F8" s="192"/>
+      <c r="I8" s="201" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="155"/>
-      <c r="K8" s="155"/>
+      <c r="J8" s="201"/>
+      <c r="K8" s="201"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="156" t="e">
+      <c r="A9" s="202" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="156"/>
-      <c r="C9" s="156"/>
-      <c r="D9" s="156"/>
-      <c r="E9" s="156"/>
-      <c r="F9" s="156"/>
-      <c r="I9" s="155" t="s">
+      <c r="B9" s="202"/>
+      <c r="C9" s="202"/>
+      <c r="D9" s="202"/>
+      <c r="E9" s="202"/>
+      <c r="F9" s="202"/>
+      <c r="I9" s="201" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="155"/>
-      <c r="K9" s="155"/>
+      <c r="J9" s="201"/>
+      <c r="K9" s="201"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="150" t="s">
+      <c r="A11" s="197" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="150" t="s">
+      <c r="B11" s="197" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="150" t="s">
+      <c r="C11" s="197" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="157" t="s">
+      <c r="D11" s="203" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="157"/>
-      <c r="F11" s="157"/>
-      <c r="G11" s="157" t="s">
+      <c r="E11" s="203"/>
+      <c r="F11" s="203"/>
+      <c r="G11" s="203" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="157"/>
-      <c r="I11" s="157"/>
-      <c r="J11" s="150" t="s">
+      <c r="H11" s="203"/>
+      <c r="I11" s="203"/>
+      <c r="J11" s="197" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="151" t="s">
+      <c r="K11" s="198" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="150"/>
-      <c r="B12" s="150"/>
-      <c r="C12" s="150"/>
+      <c r="A12" s="197"/>
+      <c r="B12" s="197"/>
+      <c r="C12" s="197"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -6609,10 +6618,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="150"/>
-      <c r="K12" s="151"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="27.6">
+      <c r="J12" s="197"/>
+      <c r="K12" s="198"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A13" s="26">
         <f>backyard!A9</f>
         <v>1</v>
@@ -6655,7 +6664,7 @@
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A14" s="26"/>
       <c r="B14" s="31"/>
       <c r="C14" s="12"/>
@@ -6668,7 +6677,7 @@
       <c r="J14" s="27"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" ht="27.6">
+    <row r="15" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A15" s="26">
         <f>backyard!A13</f>
         <v>2</v>
@@ -6711,7 +6720,7 @@
       </c>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="16" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A16" s="26"/>
       <c r="B16" s="31" t="str">
         <f>backyard!B17</f>
@@ -6736,7 +6745,7 @@
       </c>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="17" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A17" s="26"/>
       <c r="B17" s="31"/>
       <c r="C17" s="12"/>
@@ -6749,7 +6758,7 @@
       <c r="J17" s="27"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" s="1" customFormat="1" ht="41.4">
+    <row r="18" spans="1:11" s="1" customFormat="1" ht="57">
       <c r="A18" s="26">
         <f>backyard!A19</f>
         <v>3</v>
@@ -6792,7 +6801,7 @@
       </c>
       <c r="K18" s="14"/>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="19" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A19" s="26"/>
       <c r="B19" s="31" t="str">
         <f>backyard!B24</f>
@@ -6817,7 +6826,7 @@
       </c>
       <c r="K19" s="14"/>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="20" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A20" s="26"/>
       <c r="B20" s="31"/>
       <c r="C20" s="12"/>
@@ -6830,7 +6839,7 @@
       <c r="J20" s="27"/>
       <c r="K20" s="14"/>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" ht="27.6">
+    <row r="21" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A21" s="26">
         <f>backyard!A26</f>
         <v>4</v>
@@ -6873,7 +6882,7 @@
       </c>
       <c r="K21" s="14"/>
     </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="22" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A22" s="26"/>
       <c r="B22" s="31" t="str">
         <f>backyard!B29</f>
@@ -6898,7 +6907,7 @@
       </c>
       <c r="K22" s="14"/>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="23" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A23" s="26"/>
       <c r="B23" s="31"/>
       <c r="C23" s="12"/>
@@ -6911,7 +6920,7 @@
       <c r="J23" s="27"/>
       <c r="K23" s="14"/>
     </row>
-    <row r="24" spans="1:11" s="1" customFormat="1" ht="27.6">
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A24" s="26">
         <f>backyard!A31</f>
         <v>5</v>
@@ -6954,7 +6963,7 @@
       </c>
       <c r="K24" s="14"/>
     </row>
-    <row r="25" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="25" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A25" s="26"/>
       <c r="B25" s="31" t="str">
         <f>backyard!B34</f>
@@ -6979,7 +6988,7 @@
       </c>
       <c r="K25" s="14"/>
     </row>
-    <row r="26" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="26" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A26" s="26"/>
       <c r="B26" s="31"/>
       <c r="C26" s="12"/>
@@ -6992,7 +7001,7 @@
       <c r="J26" s="27"/>
       <c r="K26" s="14"/>
     </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" ht="27.6">
+    <row r="27" spans="1:11" s="1" customFormat="1" ht="42.75">
       <c r="A27" s="26">
         <f>backyard!A36</f>
         <v>6</v>
@@ -7035,7 +7044,7 @@
       </c>
       <c r="K27" s="14"/>
     </row>
-    <row r="28" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="28" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A28" s="26"/>
       <c r="B28" s="31" t="str">
         <f>backyard!B39</f>
@@ -7060,7 +7069,7 @@
       </c>
       <c r="K28" s="14"/>
     </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="29" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A29" s="26"/>
       <c r="B29" s="31"/>
       <c r="C29" s="12"/>
@@ -7073,7 +7082,7 @@
       <c r="J29" s="27"/>
       <c r="K29" s="14"/>
     </row>
-    <row r="30" spans="1:11" s="1" customFormat="1" ht="27.6">
+    <row r="30" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A30" s="26">
         <f>backyard!A41</f>
         <v>7</v>
@@ -7116,7 +7125,7 @@
       </c>
       <c r="K30" s="14"/>
     </row>
-    <row r="31" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="31" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A31" s="26"/>
       <c r="B31" s="31"/>
       <c r="C31" s="12"/>
@@ -7172,7 +7181,7 @@
       </c>
       <c r="K32" s="14"/>
     </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="33" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A33" s="26"/>
       <c r="B33" s="31" t="str">
         <f>backyard!B50</f>
@@ -7197,7 +7206,7 @@
       </c>
       <c r="K33" s="14"/>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="34" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A34" s="26"/>
       <c r="B34" s="31"/>
       <c r="C34" s="12"/>
@@ -7210,7 +7219,7 @@
       <c r="J34" s="27"/>
       <c r="K34" s="14"/>
     </row>
-    <row r="35" spans="1:11" s="1" customFormat="1" ht="27.6">
+    <row r="35" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A35" s="26">
         <f>backyard!A52</f>
         <v>9</v>
@@ -7253,7 +7262,7 @@
       </c>
       <c r="K35" s="14"/>
     </row>
-    <row r="36" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="36" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A36" s="26"/>
       <c r="B36" s="31" t="str">
         <f>backyard!B57</f>
@@ -7278,7 +7287,7 @@
       </c>
       <c r="K36" s="14"/>
     </row>
-    <row r="37" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="37" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A37" s="26"/>
       <c r="B37" s="31"/>
       <c r="C37" s="12"/>
@@ -7291,7 +7300,7 @@
       <c r="J37" s="27"/>
       <c r="K37" s="14"/>
     </row>
-    <row r="38" spans="1:11" s="1" customFormat="1" ht="25.2">
+    <row r="38" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A38" s="26">
         <f>backyard!A59</f>
         <v>10</v>
@@ -7333,7 +7342,7 @@
       </c>
       <c r="K38" s="14"/>
     </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="39" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A39" s="26"/>
       <c r="B39" s="31" t="str">
         <f>backyard!B62</f>
@@ -7358,7 +7367,7 @@
       </c>
       <c r="K39" s="14"/>
     </row>
-    <row r="40" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="40" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A40" s="26"/>
       <c r="B40" s="31"/>
       <c r="C40" s="12"/>
@@ -7371,7 +7380,7 @@
       <c r="J40" s="27"/>
       <c r="K40" s="14"/>
     </row>
-    <row r="41" spans="1:11" s="1" customFormat="1" ht="27.6">
+    <row r="41" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A41" s="26">
         <f>backyard!A64</f>
         <v>11</v>
@@ -7414,7 +7423,7 @@
       </c>
       <c r="K41" s="14"/>
     </row>
-    <row r="42" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="42" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A42" s="26"/>
       <c r="B42" s="31" t="str">
         <f>backyard!B70</f>
@@ -7439,7 +7448,7 @@
       </c>
       <c r="K42" s="14"/>
     </row>
-    <row r="43" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="43" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A43" s="26"/>
       <c r="B43" s="31"/>
       <c r="C43" s="12"/>
@@ -7452,12 +7461,12 @@
       <c r="J43" s="27"/>
       <c r="K43" s="14"/>
     </row>
-    <row r="44" spans="1:11" s="1" customFormat="1">
+    <row r="44" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A44" s="26">
         <f>backyard!A72</f>
         <v>12</v>
       </c>
-      <c r="B44" s="219" t="str">
+      <c r="B44" s="182" t="str">
         <f>backyard!B72</f>
         <v>kmnfd]sf] kfOk / KnfOaf]8{af6 kmdf{ agfpg] sfd</v>
       </c>
@@ -7495,7 +7504,7 @@
       </c>
       <c r="K44" s="14"/>
     </row>
-    <row r="45" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="45" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A45" s="26"/>
       <c r="B45" s="31" t="str">
         <f>backyard!B78</f>
@@ -7520,7 +7529,7 @@
       </c>
       <c r="K45" s="14"/>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="46" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A46" s="26"/>
       <c r="B46" s="31"/>
       <c r="C46" s="12"/>
@@ -7533,12 +7542,12 @@
       <c r="J46" s="27"/>
       <c r="K46" s="14"/>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" ht="27.6">
+    <row r="47" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A47" s="26">
         <f>backyard!A80</f>
         <v>13</v>
       </c>
-      <c r="B47" s="219" t="str">
+      <c r="B47" s="182" t="str">
         <f>backyard!B80</f>
         <v>d]lzgsf] k|of]u u/L ;'k/ :6«Sr/df l;d]G6 s+lqm6 ug]{ sfd -!M!=%M#_</v>
       </c>
@@ -7576,7 +7585,7 @@
       </c>
       <c r="K47" s="14"/>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="48" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A48" s="26"/>
       <c r="B48" s="31" t="str">
         <f>backyard!B85</f>
@@ -7601,7 +7610,7 @@
       </c>
       <c r="K48" s="14"/>
     </row>
-    <row r="49" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="49" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A49" s="26"/>
       <c r="B49" s="31"/>
       <c r="C49" s="12"/>
@@ -7614,12 +7623,12 @@
       <c r="J49" s="27"/>
       <c r="K49" s="14"/>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" ht="27.6">
+    <row r="50" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A50" s="26">
         <f>backyard!A87</f>
         <v>14</v>
       </c>
-      <c r="B50" s="219" t="str">
+      <c r="B50" s="182" t="str">
         <f>backyard!B87</f>
         <v>ljleGg ;fO{hsf] kmnfd] PËn km]lj|s]zg u/L k|fOd/ k]G6 ;lxt ug]{</v>
       </c>
@@ -7657,7 +7666,7 @@
       </c>
       <c r="K50" s="14"/>
     </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="51" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A51" s="26"/>
       <c r="B51" s="31" t="str">
         <f>backyard!B101</f>
@@ -7682,7 +7691,7 @@
       </c>
       <c r="K51" s="14"/>
     </row>
-    <row r="52" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="52" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A52" s="26"/>
       <c r="B52" s="31"/>
       <c r="C52" s="12"/>
@@ -7722,7 +7731,7 @@
       </c>
       <c r="G53" s="12">
         <f>V!G170</f>
-        <v>187.88588744285281</v>
+        <v>128.22878564462053</v>
       </c>
       <c r="H53" s="12">
         <f>V!I170</f>
@@ -7730,15 +7739,15 @@
       </c>
       <c r="I53" s="12">
         <f t="shared" ref="I53" si="38">G53*H53</f>
-        <v>76255.366277556241</v>
+        <v>52042.934941725689</v>
       </c>
       <c r="J53" s="27">
         <f t="shared" ref="J53:J54" si="39">I53-F53</f>
-        <v>39952.60671052432</v>
+        <v>15740.175374693768</v>
       </c>
       <c r="K53" s="14"/>
     </row>
-    <row r="54" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="54" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A54" s="26"/>
       <c r="B54" s="31" t="str">
         <f>backyard!B116</f>
@@ -7755,15 +7764,15 @@
       <c r="H54" s="12"/>
       <c r="I54" s="12">
         <f>V!J171</f>
-        <v>2727.3628152736983</v>
+        <v>1861.3767461444502</v>
       </c>
       <c r="J54" s="27">
         <f t="shared" si="39"/>
-        <v>1428.9519444300342</v>
+        <v>562.96587530078614</v>
       </c>
       <c r="K54" s="14"/>
     </row>
-    <row r="55" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="55" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A55" s="26"/>
       <c r="B55" s="31"/>
       <c r="C55" s="12"/>
@@ -7776,7 +7785,7 @@
       <c r="J55" s="27"/>
       <c r="K55" s="14"/>
     </row>
-    <row r="56" spans="1:11" s="1" customFormat="1" ht="27.6">
+    <row r="56" spans="1:11" s="1" customFormat="1" ht="28.5">
       <c r="A56" s="26">
         <f>backyard!A118</f>
         <v>16</v>
@@ -7819,7 +7828,7 @@
       </c>
       <c r="K56" s="14"/>
     </row>
-    <row r="57" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="57" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A57" s="26"/>
       <c r="B57" s="31" t="str">
         <f>backyard!B121</f>
@@ -7844,7 +7853,7 @@
       </c>
       <c r="K57" s="14"/>
     </row>
-    <row r="58" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="58" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A58" s="26"/>
       <c r="B58" s="31"/>
       <c r="C58" s="12"/>
@@ -7857,7 +7866,7 @@
       <c r="J58" s="27"/>
       <c r="K58" s="14"/>
     </row>
-    <row r="59" spans="1:11" s="1" customFormat="1" ht="52.2">
+    <row r="59" spans="1:11" s="1" customFormat="1" ht="54">
       <c r="A59" s="26">
         <f>backyard!A123</f>
         <v>17</v>
@@ -7899,7 +7908,7 @@
       </c>
       <c r="K59" s="14"/>
     </row>
-    <row r="60" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="60" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A60" s="26"/>
       <c r="B60" s="31"/>
       <c r="C60" s="12"/>
@@ -7921,7 +7930,7 @@
       </c>
       <c r="K60" s="14"/>
     </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="61" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A61" s="26"/>
       <c r="B61" s="31"/>
       <c r="C61" s="12"/>
@@ -7977,7 +7986,7 @@
       </c>
       <c r="K62" s="14"/>
     </row>
-    <row r="63" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="63" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A63" s="26"/>
       <c r="B63" s="31" t="str">
         <f>backyard!B136</f>
@@ -8002,7 +8011,7 @@
       </c>
       <c r="K63" s="14"/>
     </row>
-    <row r="64" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="64" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A64" s="26"/>
       <c r="B64" s="31"/>
       <c r="C64" s="12"/>
@@ -8015,7 +8024,7 @@
       <c r="J64" s="27"/>
       <c r="K64" s="14"/>
     </row>
-    <row r="65" spans="1:11" s="1" customFormat="1" ht="41.4">
+    <row r="65" spans="1:11" s="1" customFormat="1" ht="42.75">
       <c r="A65" s="26">
         <f>backyard!A138</f>
         <v>19</v>
@@ -8058,7 +8067,7 @@
       </c>
       <c r="K65" s="14"/>
     </row>
-    <row r="66" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="66" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A66" s="26"/>
       <c r="B66" s="31"/>
       <c r="C66" s="12"/>
@@ -8071,7 +8080,7 @@
       <c r="J66" s="27"/>
       <c r="K66" s="14"/>
     </row>
-    <row r="67" spans="1:11" s="1" customFormat="1" ht="15.6">
+    <row r="67" spans="1:11" s="1" customFormat="1" ht="15.75">
       <c r="A67" s="26">
         <f>backyard!A143</f>
         <v>20</v>
@@ -8199,16 +8208,23 @@
       <c r="H71" s="7"/>
       <c r="I71" s="7">
         <f>SUM(I13:I69)</f>
-        <v>450558.50226700824</v>
+        <v>425480.08486204845</v>
       </c>
       <c r="J71" s="13">
         <f>I71-F71</f>
-        <v>-114414.51724356477</v>
+        <v>-139492.93464852456</v>
       </c>
       <c r="K71" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -8222,13 +8238,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8250,21 +8259,21 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="63"/>
-    <col min="2" max="2" width="11.44140625" style="63" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="63" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="63"/>
-    <col min="6" max="6" width="10.44140625" style="63" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" style="63" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="63" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="63"/>
+    <col min="1" max="1" width="8.85546875" style="63"/>
+    <col min="2" max="2" width="11.42578125" style="63" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="63" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="63"/>
+    <col min="6" max="6" width="10.42578125" style="63" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="63" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" style="63" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="63"/>
     <col min="10" max="10" width="12" style="63" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="63"/>
+    <col min="11" max="16384" width="8.85546875" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21">
+    <row r="1" spans="1:10" ht="20.25">
       <c r="A1" s="61" t="e">
         <f>+#REF!+1</f>
         <v>#REF!</v>
@@ -8289,33 +8298,33 @@
       <c r="G2" s="65"/>
       <c r="H2" s="65"/>
     </row>
-    <row r="3" spans="1:10" ht="17.399999999999999">
+    <row r="3" spans="1:10" ht="18">
       <c r="A3" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="B3" s="167" t="s">
+      <c r="B3" s="218" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167"/>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="167"/>
-    </row>
-    <row r="4" spans="1:10" ht="15">
+      <c r="C3" s="218"/>
+      <c r="D3" s="218"/>
+      <c r="E3" s="218"/>
+      <c r="F3" s="218"/>
+      <c r="G3" s="218"/>
+      <c r="H3" s="218"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75">
       <c r="A4" s="67"/>
-      <c r="B4" s="168" t="s">
+      <c r="B4" s="219" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="168"/>
-      <c r="D4" s="168"/>
-      <c r="E4" s="168"/>
-      <c r="F4" s="168"/>
-      <c r="G4" s="168"/>
-      <c r="H4" s="168"/>
-    </row>
-    <row r="5" spans="1:10" ht="32.4">
+      <c r="C4" s="219"/>
+      <c r="D4" s="219"/>
+      <c r="E4" s="219"/>
+      <c r="F4" s="219"/>
+      <c r="G4" s="219"/>
+      <c r="H4" s="219"/>
+    </row>
+    <row r="5" spans="1:10" ht="31.5">
       <c r="A5" s="67"/>
       <c r="B5" s="68" t="s">
         <v>52</v>
@@ -8339,9 +8348,9 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18">
+    <row r="6" spans="1:10" ht="17.25">
       <c r="A6" s="67"/>
-      <c r="B6" s="169" t="s">
+      <c r="B6" s="220" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="68" t="s">
@@ -8362,9 +8371,9 @@
       </c>
       <c r="H6" s="73"/>
     </row>
-    <row r="7" spans="1:10" ht="18">
+    <row r="7" spans="1:10" ht="17.25">
       <c r="A7" s="67"/>
-      <c r="B7" s="170"/>
+      <c r="B7" s="221"/>
       <c r="C7" s="70" t="s">
         <v>62</v>
       </c>
@@ -8386,9 +8395,9 @@
         <v>3065</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="43.8">
+    <row r="8" spans="1:10" ht="45">
       <c r="A8" s="67"/>
-      <c r="B8" s="169" t="s">
+      <c r="B8" s="220" t="s">
         <v>63</v>
       </c>
       <c r="C8" s="74" t="s">
@@ -8409,9 +8418,9 @@
       </c>
       <c r="H8" s="73"/>
     </row>
-    <row r="9" spans="1:10" ht="18">
+    <row r="9" spans="1:10" ht="17.25">
       <c r="A9" s="67"/>
-      <c r="B9" s="169"/>
+      <c r="B9" s="220"/>
       <c r="C9" s="70" t="s">
         <v>66</v>
       </c>
@@ -8430,9 +8439,9 @@
       </c>
       <c r="H9" s="76"/>
     </row>
-    <row r="10" spans="1:10" ht="18">
+    <row r="10" spans="1:10" ht="17.25">
       <c r="A10" s="67"/>
-      <c r="B10" s="169"/>
+      <c r="B10" s="220"/>
       <c r="C10" s="70" t="s">
         <v>68</v>
       </c>
@@ -8455,9 +8464,9 @@
         <v>99000</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="18">
+    <row r="11" spans="1:10" ht="17.25">
       <c r="A11" s="67"/>
-      <c r="B11" s="169"/>
+      <c r="B11" s="220"/>
       <c r="C11" s="70" t="s">
         <v>70</v>
       </c>
@@ -8477,9 +8486,9 @@
       </c>
       <c r="H11" s="76"/>
     </row>
-    <row r="12" spans="1:10" ht="18">
+    <row r="12" spans="1:10" ht="17.25">
       <c r="A12" s="67"/>
-      <c r="B12" s="169"/>
+      <c r="B12" s="220"/>
       <c r="C12" s="70" t="s">
         <v>71</v>
       </c>
@@ -8503,9 +8512,9 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="18">
+    <row r="13" spans="1:10" ht="17.25">
       <c r="A13" s="67"/>
-      <c r="B13" s="169"/>
+      <c r="B13" s="220"/>
       <c r="C13" s="70" t="s">
         <v>73</v>
       </c>
@@ -8528,7 +8537,7 @@
         <v>5504.3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="18">
+    <row r="14" spans="1:10" ht="17.25">
       <c r="A14" s="67"/>
       <c r="B14" s="67"/>
       <c r="C14" s="67"/>
@@ -8543,7 +8552,7 @@
         <v>8569.2999999999993</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="18">
+    <row r="15" spans="1:10" ht="17.25">
       <c r="B15" s="82" t="s">
         <v>76</v>
       </c>
@@ -8557,7 +8566,7 @@
         <v>1285.3900000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="18">
+    <row r="16" spans="1:10" ht="17.25">
       <c r="A16" s="83" t="s">
         <v>78</v>
       </c>
@@ -8579,7 +8588,7 @@
         <v>9854.6899999999987</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="18">
+    <row r="17" spans="1:8" ht="17.25">
       <c r="A17" s="83"/>
       <c r="B17" s="84"/>
       <c r="C17" s="67"/>
@@ -8594,7 +8603,7 @@
         <v>1094.9655555555555</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="18">
+    <row r="18" spans="1:8" ht="17.25">
       <c r="A18" s="83"/>
       <c r="B18" s="84"/>
       <c r="C18" s="67"/>
@@ -8609,7 +8618,7 @@
         <v>952.14396135265702</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="18">
+    <row r="19" spans="1:8" ht="17.25">
       <c r="A19" s="83"/>
       <c r="B19" s="85" t="s">
         <v>83</v>
@@ -8621,43 +8630,43 @@
       <c r="G19" s="80"/>
       <c r="H19" s="84"/>
     </row>
-    <row r="22" spans="1:8" s="93" customFormat="1" ht="21">
+    <row r="22" spans="1:8" s="93" customFormat="1" ht="20.25">
       <c r="A22" s="92">
         <f>+A9+1</f>
         <v>1</v>
       </c>
-      <c r="B22" s="171"/>
-      <c r="C22" s="171"/>
-      <c r="D22" s="171"/>
-      <c r="E22" s="171"/>
-      <c r="F22" s="171"/>
-      <c r="G22" s="171"/>
-      <c r="H22" s="171"/>
-    </row>
-    <row r="23" spans="1:8" s="93" customFormat="1" ht="19.8">
+      <c r="B22" s="210"/>
+      <c r="C22" s="210"/>
+      <c r="D22" s="210"/>
+      <c r="E22" s="210"/>
+      <c r="F22" s="210"/>
+      <c r="G22" s="210"/>
+      <c r="H22" s="210"/>
+    </row>
+    <row r="23" spans="1:8" s="93" customFormat="1" ht="19.5">
       <c r="A23" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="171" t="s">
+      <c r="B23" s="210" t="s">
         <v>116</v>
       </c>
-      <c r="C23" s="171"/>
-      <c r="D23" s="171"/>
-      <c r="E23" s="171"/>
-      <c r="F23" s="171"/>
-      <c r="G23" s="171"/>
-      <c r="H23" s="171"/>
+      <c r="C23" s="210"/>
+      <c r="D23" s="210"/>
+      <c r="E23" s="210"/>
+      <c r="F23" s="210"/>
+      <c r="G23" s="210"/>
+      <c r="H23" s="210"/>
     </row>
     <row r="24" spans="1:8" s="93" customFormat="1" ht="15">
-      <c r="B24" s="173" t="s">
+      <c r="B24" s="211" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="173"/>
-      <c r="D24" s="173"/>
-      <c r="E24" s="173"/>
-      <c r="F24" s="173"/>
-      <c r="G24" s="173"/>
-      <c r="H24" s="173"/>
+      <c r="C24" s="211"/>
+      <c r="D24" s="211"/>
+      <c r="E24" s="211"/>
+      <c r="F24" s="211"/>
+      <c r="G24" s="211"/>
+      <c r="H24" s="211"/>
     </row>
     <row r="25" spans="1:8" s="93" customFormat="1" ht="30" customHeight="1">
       <c r="B25" s="95" t="s">
@@ -8683,7 +8692,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" s="93" customFormat="1" ht="24.75" customHeight="1">
-      <c r="B26" s="174" t="s">
+      <c r="B26" s="212" t="s">
         <v>59</v>
       </c>
       <c r="C26" s="96" t="s">
@@ -8704,8 +8713,8 @@
       </c>
       <c r="H26" s="101"/>
     </row>
-    <row r="27" spans="1:8" s="93" customFormat="1" ht="18">
-      <c r="B27" s="175"/>
+    <row r="27" spans="1:8" s="93" customFormat="1" ht="17.25">
+      <c r="B27" s="213"/>
       <c r="C27" s="102" t="s">
         <v>62</v>
       </c>
@@ -8727,8 +8736,8 @@
         <v>44714</v>
       </c>
     </row>
-    <row r="28" spans="1:8" s="93" customFormat="1" ht="18">
-      <c r="B28" s="176" t="s">
+    <row r="28" spans="1:8" s="93" customFormat="1" ht="17.25">
+      <c r="B28" s="214" t="s">
         <v>63</v>
       </c>
       <c r="C28" s="98" t="s">
@@ -8749,8 +8758,8 @@
       </c>
       <c r="H28" s="101"/>
     </row>
-    <row r="29" spans="1:8" s="93" customFormat="1" ht="18">
-      <c r="B29" s="177"/>
+    <row r="29" spans="1:8" s="93" customFormat="1" ht="17.25">
+      <c r="B29" s="215"/>
       <c r="C29" s="102" t="s">
         <v>106</v>
       </c>
@@ -8770,8 +8779,8 @@
       </c>
       <c r="H29" s="106"/>
     </row>
-    <row r="30" spans="1:8" s="93" customFormat="1" ht="27.6">
-      <c r="B30" s="177"/>
+    <row r="30" spans="1:8" s="93" customFormat="1" ht="27.75">
+      <c r="B30" s="215"/>
       <c r="C30" s="109" t="s">
         <v>117</v>
       </c>
@@ -8791,8 +8800,8 @@
       </c>
       <c r="H30" s="106"/>
     </row>
-    <row r="31" spans="1:8" s="93" customFormat="1" ht="18">
-      <c r="B31" s="178"/>
+    <row r="31" spans="1:8" s="93" customFormat="1" ht="17.25">
+      <c r="B31" s="216"/>
       <c r="C31" s="104" t="s">
         <v>108</v>
       </c>
@@ -8815,7 +8824,7 @@
         <v>36690.270000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="93" customFormat="1" ht="18">
+    <row r="32" spans="1:8" s="93" customFormat="1" ht="17.25">
       <c r="F32" s="113" t="s">
         <v>75</v>
       </c>
@@ -8825,7 +8834,7 @@
         <v>81404.27</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="93" customFormat="1" ht="18">
+    <row r="33" spans="1:8" s="93" customFormat="1" ht="17.25">
       <c r="B33" s="93" t="s">
         <v>110</v>
       </c>
@@ -8869,16 +8878,16 @@
       </c>
     </row>
     <row r="36" spans="1:8" s="93" customFormat="1" ht="12" customHeight="1">
-      <c r="A36" s="179" t="s">
+      <c r="A36" s="217" t="s">
         <v>118</v>
       </c>
-      <c r="B36" s="179"/>
-      <c r="C36" s="179"/>
-      <c r="D36" s="179"/>
-      <c r="E36" s="179"/>
-      <c r="F36" s="179"/>
-      <c r="G36" s="179"/>
-      <c r="H36" s="179"/>
+      <c r="B36" s="217"/>
+      <c r="C36" s="217"/>
+      <c r="D36" s="217"/>
+      <c r="E36" s="217"/>
+      <c r="F36" s="217"/>
+      <c r="G36" s="217"/>
+      <c r="H36" s="217"/>
     </row>
     <row r="37" spans="1:8" s="93" customFormat="1" ht="12" customHeight="1">
       <c r="B37" s="118" t="s">
@@ -8886,16 +8895,16 @@
       </c>
     </row>
     <row r="38" spans="1:8" s="93" customFormat="1" ht="12" customHeight="1">
-      <c r="A38" s="172" t="s">
+      <c r="A38" s="209" t="s">
         <v>112</v>
       </c>
-      <c r="B38" s="172"/>
-      <c r="C38" s="172"/>
-      <c r="D38" s="172"/>
-      <c r="E38" s="172"/>
-      <c r="F38" s="172"/>
-      <c r="G38" s="172"/>
-      <c r="H38" s="172"/>
+      <c r="B38" s="209"/>
+      <c r="C38" s="209"/>
+      <c r="D38" s="209"/>
+      <c r="E38" s="209"/>
+      <c r="F38" s="209"/>
+      <c r="G38" s="209"/>
+      <c r="H38" s="209"/>
     </row>
     <row r="39" spans="1:8" s="93" customFormat="1" ht="12" customHeight="1">
       <c r="B39" s="118" t="s">
@@ -8903,16 +8912,16 @@
       </c>
     </row>
     <row r="40" spans="1:8" s="93" customFormat="1" ht="12" customHeight="1">
-      <c r="A40" s="172" t="s">
+      <c r="A40" s="209" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="172"/>
-      <c r="C40" s="172"/>
-      <c r="D40" s="172"/>
-      <c r="E40" s="172"/>
-      <c r="F40" s="172"/>
-      <c r="G40" s="172"/>
-      <c r="H40" s="172"/>
+      <c r="B40" s="209"/>
+      <c r="C40" s="209"/>
+      <c r="D40" s="209"/>
+      <c r="E40" s="209"/>
+      <c r="F40" s="209"/>
+      <c r="G40" s="209"/>
+      <c r="H40" s="209"/>
     </row>
     <row r="41" spans="1:8" s="93" customFormat="1" ht="12" customHeight="1">
       <c r="B41" s="118" t="s">
@@ -8924,6 +8933,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="B22:H22"/>
     <mergeCell ref="A38:H38"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="B23:H23"/>
@@ -8931,11 +8945,6 @@
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="A36:H36"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B22:H22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8946,131 +8955,131 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V267"/>
   <sheetViews>
-    <sheetView topLeftCell="A138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G171" sqref="G171"/>
+    <sheetView tabSelected="1" topLeftCell="A199" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B206" sqref="B206"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="188" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
-      <c r="I1" s="159"/>
-      <c r="J1" s="159"/>
-      <c r="K1" s="159"/>
-    </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.8">
-      <c r="A2" s="160" t="s">
+      <c r="B1" s="188"/>
+      <c r="C1" s="188"/>
+      <c r="D1" s="188"/>
+      <c r="E1" s="188"/>
+      <c r="F1" s="188"/>
+      <c r="G1" s="188"/>
+      <c r="H1" s="188"/>
+      <c r="I1" s="188"/>
+      <c r="J1" s="188"/>
+      <c r="K1" s="188"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="22.5">
+      <c r="A2" s="189" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="160"/>
-      <c r="G2" s="160"/>
-      <c r="H2" s="160"/>
-      <c r="I2" s="160"/>
-      <c r="J2" s="160"/>
-      <c r="K2" s="160"/>
+      <c r="B2" s="189"/>
+      <c r="C2" s="189"/>
+      <c r="D2" s="189"/>
+      <c r="E2" s="189"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="189"/>
+      <c r="H2" s="189"/>
+      <c r="I2" s="189"/>
+      <c r="J2" s="189"/>
+      <c r="K2" s="189"/>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="190" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="148"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="148"/>
-      <c r="F3" s="148"/>
-      <c r="G3" s="148"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="K3" s="148"/>
+      <c r="B3" s="190"/>
+      <c r="C3" s="190"/>
+      <c r="D3" s="190"/>
+      <c r="E3" s="190"/>
+      <c r="F3" s="190"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="190"/>
+      <c r="I3" s="190"/>
+      <c r="J3" s="190"/>
+      <c r="K3" s="190"/>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1">
-      <c r="A4" s="148" t="s">
+      <c r="A4" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="148"/>
-      <c r="C4" s="148"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="148"/>
-      <c r="F4" s="148"/>
-      <c r="G4" s="148"/>
-      <c r="H4" s="148"/>
-      <c r="I4" s="148"/>
-      <c r="J4" s="148"/>
-      <c r="K4" s="148"/>
-    </row>
-    <row r="5" spans="1:14" ht="17.399999999999999">
-      <c r="A5" s="161" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="161"/>
-      <c r="C5" s="161"/>
-      <c r="D5" s="161"/>
-      <c r="E5" s="161"/>
-      <c r="F5" s="161"/>
-      <c r="G5" s="161"/>
-      <c r="H5" s="161"/>
-      <c r="I5" s="161"/>
-      <c r="J5" s="161"/>
-      <c r="K5" s="161"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.6">
-      <c r="A6" s="152" t="s">
+      <c r="B4" s="190"/>
+      <c r="C4" s="190"/>
+      <c r="D4" s="190"/>
+      <c r="E4" s="190"/>
+      <c r="F4" s="190"/>
+      <c r="G4" s="190"/>
+      <c r="H4" s="190"/>
+      <c r="I4" s="190"/>
+      <c r="J4" s="190"/>
+      <c r="K4" s="190"/>
+    </row>
+    <row r="5" spans="1:14" ht="18.75">
+      <c r="A5" s="191" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="191"/>
+      <c r="C5" s="191"/>
+      <c r="D5" s="191"/>
+      <c r="E5" s="191"/>
+      <c r="F5" s="191"/>
+      <c r="G5" s="191"/>
+      <c r="H5" s="191"/>
+      <c r="I5" s="191"/>
+      <c r="J5" s="191"/>
+      <c r="K5" s="191"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75">
+      <c r="A6" s="192" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="152"/>
-      <c r="C6" s="152"/>
-      <c r="D6" s="152"/>
-      <c r="E6" s="152"/>
-      <c r="F6" s="152"/>
+      <c r="B6" s="192"/>
+      <c r="C6" s="192"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="192"/>
+      <c r="F6" s="192"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="158" t="s">
+      <c r="H6" s="193" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="158"/>
-      <c r="J6" s="158"/>
-      <c r="K6" s="158"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.6">
-      <c r="A7" s="162" t="s">
+      <c r="I6" s="193"/>
+      <c r="J6" s="193"/>
+      <c r="K6" s="193"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75">
+      <c r="A7" s="194" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="162"/>
-      <c r="C7" s="162"/>
-      <c r="D7" s="162"/>
-      <c r="E7" s="162"/>
-      <c r="F7" s="162"/>
+      <c r="B7" s="194"/>
+      <c r="C7" s="194"/>
+      <c r="D7" s="194"/>
+      <c r="E7" s="194"/>
+      <c r="F7" s="194"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="163" t="s">
+      <c r="H7" s="195" t="s">
         <v>158</v>
       </c>
-      <c r="I7" s="163"/>
-      <c r="J7" s="163"/>
-      <c r="K7" s="163"/>
+      <c r="I7" s="195"/>
+      <c r="J7" s="195"/>
+      <c r="K7" s="195"/>
     </row>
     <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" s="4" t="s">
@@ -9107,7 +9116,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="27.6">
+    <row r="9" spans="1:14" ht="28.5">
       <c r="A9" s="18">
         <v>1</v>
       </c>
@@ -9151,7 +9160,7 @@
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
-      <c r="K10" s="60"/>
+      <c r="K10" s="222"/>
       <c r="N10">
         <f>5.84+1.76</f>
         <v>7.6</v>
@@ -9182,7 +9191,7 @@
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
       <c r="J11" s="38"/>
-      <c r="K11" s="60"/>
+      <c r="K11" s="222"/>
     </row>
     <row r="12" spans="1:14" ht="15" customHeight="1">
       <c r="A12" s="18"/>
@@ -9209,7 +9218,7 @@
       <c r="H12" s="38"/>
       <c r="I12" s="38"/>
       <c r="J12" s="38"/>
-      <c r="K12" s="60"/>
+      <c r="K12" s="222"/>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1">
       <c r="A13" s="18"/>
@@ -9236,7 +9245,7 @@
       <c r="H13" s="38"/>
       <c r="I13" s="38"/>
       <c r="J13" s="38"/>
-      <c r="K13" s="60"/>
+      <c r="K13" s="222"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1">
       <c r="A14" s="18"/>
@@ -9263,7 +9272,7 @@
       <c r="H14" s="38"/>
       <c r="I14" s="38"/>
       <c r="J14" s="38"/>
-      <c r="K14" s="60"/>
+      <c r="K14" s="222"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1">
       <c r="A15" s="18"/>
@@ -9303,7 +9312,7 @@
       <c r="J16" s="40"/>
       <c r="K16" s="21"/>
     </row>
-    <row r="17" spans="1:14" ht="27.6">
+    <row r="17" spans="1:14" ht="28.5">
       <c r="A17" s="18">
         <v>2</v>
       </c>
@@ -9346,7 +9355,7 @@
       <c r="H18" s="38"/>
       <c r="I18" s="38"/>
       <c r="J18" s="38"/>
-      <c r="K18" s="60"/>
+      <c r="K18" s="222"/>
       <c r="N18">
         <f>5.84+1.76</f>
         <v>7.6</v>
@@ -9376,7 +9385,7 @@
       <c r="H19" s="38"/>
       <c r="I19" s="38"/>
       <c r="J19" s="38"/>
-      <c r="K19" s="60"/>
+      <c r="K19" s="222"/>
     </row>
     <row r="20" spans="1:14" ht="15" customHeight="1">
       <c r="A20" s="18"/>
@@ -9402,7 +9411,7 @@
       <c r="H20" s="38"/>
       <c r="I20" s="38"/>
       <c r="J20" s="38"/>
-      <c r="K20" s="60"/>
+      <c r="K20" s="222"/>
     </row>
     <row r="21" spans="1:14" ht="15" customHeight="1">
       <c r="A21" s="18"/>
@@ -9428,7 +9437,7 @@
       <c r="H21" s="38"/>
       <c r="I21" s="38"/>
       <c r="J21" s="38"/>
-      <c r="K21" s="60"/>
+      <c r="K21" s="222"/>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1">
       <c r="A22" s="18"/>
@@ -9454,7 +9463,7 @@
       <c r="H22" s="38"/>
       <c r="I22" s="38"/>
       <c r="J22" s="38"/>
-      <c r="K22" s="60"/>
+      <c r="K22" s="222"/>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1">
       <c r="A23" s="18"/>
@@ -9480,7 +9489,7 @@
       <c r="H23" s="38"/>
       <c r="I23" s="38"/>
       <c r="J23" s="38"/>
-      <c r="K23" s="60"/>
+      <c r="K23" s="222"/>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1">
       <c r="A24" s="18"/>
@@ -9506,7 +9515,7 @@
       <c r="H24" s="38"/>
       <c r="I24" s="38"/>
       <c r="J24" s="38"/>
-      <c r="K24" s="60"/>
+      <c r="K24" s="222"/>
     </row>
     <row r="25" spans="1:14" ht="15" customHeight="1">
       <c r="A25" s="18"/>
@@ -9532,7 +9541,7 @@
       <c r="H25" s="38"/>
       <c r="I25" s="38"/>
       <c r="J25" s="38"/>
-      <c r="K25" s="60"/>
+      <c r="K25" s="222"/>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1">
       <c r="A26" s="18"/>
@@ -9558,7 +9567,7 @@
       <c r="H26" s="38"/>
       <c r="I26" s="38"/>
       <c r="J26" s="38"/>
-      <c r="K26" s="60"/>
+      <c r="K26" s="222"/>
     </row>
     <row r="27" spans="1:14" ht="15" customHeight="1">
       <c r="A27" s="18"/>
@@ -9584,7 +9593,7 @@
       <c r="H27" s="38"/>
       <c r="I27" s="38"/>
       <c r="J27" s="38"/>
-      <c r="K27" s="60"/>
+      <c r="K27" s="222"/>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1">
       <c r="A28" s="18"/>
@@ -9610,7 +9619,7 @@
       <c r="H28" s="38"/>
       <c r="I28" s="38"/>
       <c r="J28" s="38"/>
-      <c r="K28" s="60"/>
+      <c r="K28" s="222"/>
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1">
       <c r="A29" s="18"/>
@@ -9636,7 +9645,7 @@
       <c r="H29" s="38"/>
       <c r="I29" s="38"/>
       <c r="J29" s="38"/>
-      <c r="K29" s="60"/>
+      <c r="K29" s="222"/>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1">
       <c r="A30" s="18"/>
@@ -9662,7 +9671,7 @@
       <c r="H30" s="38"/>
       <c r="I30" s="38"/>
       <c r="J30" s="38"/>
-      <c r="K30" s="60"/>
+      <c r="K30" s="222"/>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1">
       <c r="A31" s="18"/>
@@ -9688,7 +9697,7 @@
       <c r="H31" s="38"/>
       <c r="I31" s="38"/>
       <c r="J31" s="38"/>
-      <c r="K31" s="60"/>
+      <c r="K31" s="222"/>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1">
       <c r="A32" s="18"/>
@@ -9716,7 +9725,7 @@
       <c r="H32" s="38"/>
       <c r="I32" s="38"/>
       <c r="J32" s="38"/>
-      <c r="K32" s="60"/>
+      <c r="K32" s="222"/>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1">
       <c r="A33" s="18"/>
@@ -9742,7 +9751,7 @@
       <c r="H33" s="38"/>
       <c r="I33" s="38"/>
       <c r="J33" s="38"/>
-      <c r="K33" s="60"/>
+      <c r="K33" s="222"/>
     </row>
     <row r="34" spans="1:14" ht="15" customHeight="1">
       <c r="A34" s="18"/>
@@ -9768,7 +9777,7 @@
       <c r="H34" s="38"/>
       <c r="I34" s="38"/>
       <c r="J34" s="38"/>
-      <c r="K34" s="60"/>
+      <c r="K34" s="222"/>
     </row>
     <row r="35" spans="1:14" ht="15" customHeight="1">
       <c r="A35" s="18"/>
@@ -9794,7 +9803,7 @@
       <c r="H35" s="38"/>
       <c r="I35" s="38"/>
       <c r="J35" s="38"/>
-      <c r="K35" s="60"/>
+      <c r="K35" s="222"/>
     </row>
     <row r="36" spans="1:14" ht="15" customHeight="1">
       <c r="A36" s="18"/>
@@ -9818,7 +9827,7 @@
       <c r="H36" s="38"/>
       <c r="I36" s="38"/>
       <c r="J36" s="38"/>
-      <c r="K36" s="60"/>
+      <c r="K36" s="222"/>
     </row>
     <row r="37" spans="1:14" ht="15" customHeight="1">
       <c r="A37" s="18"/>
@@ -9842,7 +9851,7 @@
       <c r="H37" s="38"/>
       <c r="I37" s="38"/>
       <c r="J37" s="38"/>
-      <c r="K37" s="60"/>
+      <c r="K37" s="222"/>
     </row>
     <row r="38" spans="1:14" ht="15" customHeight="1">
       <c r="A38" s="18"/>
@@ -9900,8 +9909,8 @@
       <c r="J40" s="40"/>
       <c r="K40" s="21"/>
     </row>
-    <row r="41" spans="1:14" s="1" customFormat="1" ht="55.2">
-      <c r="A41" s="182">
+    <row r="41" spans="1:14" s="1" customFormat="1" ht="57">
+      <c r="A41" s="145">
         <v>3</v>
       </c>
       <c r="B41" s="59" t="s">
@@ -9941,7 +9950,7 @@
       <c r="H42" s="38"/>
       <c r="I42" s="38"/>
       <c r="J42" s="38"/>
-      <c r="K42" s="60"/>
+      <c r="K42" s="222"/>
       <c r="N42">
         <f>5.84+1.76</f>
         <v>7.6</v>
@@ -9969,7 +9978,7 @@
       <c r="H43" s="38"/>
       <c r="I43" s="38"/>
       <c r="J43" s="38"/>
-      <c r="K43" s="60"/>
+      <c r="K43" s="222"/>
       <c r="N43">
         <f>3.87+1.86</f>
         <v>5.73</v>
@@ -9997,7 +10006,7 @@
       <c r="H44" s="38"/>
       <c r="I44" s="38"/>
       <c r="J44" s="38"/>
-      <c r="K44" s="60"/>
+      <c r="K44" s="222"/>
     </row>
     <row r="45" spans="1:14" ht="15" customHeight="1">
       <c r="A45" s="18"/>
@@ -10055,7 +10064,7 @@
       <c r="J47" s="40"/>
       <c r="K47" s="21"/>
     </row>
-    <row r="48" spans="1:14" ht="27.6">
+    <row r="48" spans="1:14" ht="28.5">
       <c r="A48" s="18">
         <v>4</v>
       </c>
@@ -10096,7 +10105,7 @@
       <c r="H49" s="38"/>
       <c r="I49" s="38"/>
       <c r="J49" s="38"/>
-      <c r="K49" s="60"/>
+      <c r="K49" s="222"/>
       <c r="N49">
         <f>5.84+1.76</f>
         <v>7.6</v>
@@ -10158,8 +10167,8 @@
       <c r="J52" s="40"/>
       <c r="K52" s="21"/>
     </row>
-    <row r="53" spans="1:19" ht="27.6">
-      <c r="A53" s="181">
+    <row r="53" spans="1:19" ht="28.5">
+      <c r="A53" s="144">
         <v>5</v>
       </c>
       <c r="B53" s="59" t="s">
@@ -10196,7 +10205,7 @@
       <c r="H54" s="38"/>
       <c r="I54" s="38"/>
       <c r="J54" s="38"/>
-      <c r="K54" s="60"/>
+      <c r="K54" s="222"/>
       <c r="N54">
         <f>5.84+1.76</f>
         <v>7.6</v>
@@ -10258,7 +10267,7 @@
       <c r="J57" s="40"/>
       <c r="K57" s="21"/>
     </row>
-    <row r="58" spans="1:19" ht="41.4">
+    <row r="58" spans="1:19" ht="42.75">
       <c r="A58" s="18">
         <v>6</v>
       </c>
@@ -10300,7 +10309,7 @@
       <c r="H59" s="38"/>
       <c r="I59" s="38"/>
       <c r="J59" s="38"/>
-      <c r="K59" s="60"/>
+      <c r="K59" s="222"/>
       <c r="N59">
         <f>5.84+1.76</f>
         <v>7.6</v>
@@ -10362,8 +10371,8 @@
       <c r="J62" s="40"/>
       <c r="K62" s="21"/>
     </row>
-    <row r="63" spans="1:19" ht="30.6">
-      <c r="A63" s="181">
+    <row r="63" spans="1:19" ht="30.75">
+      <c r="A63" s="144">
         <v>7</v>
       </c>
       <c r="B63" s="86" t="s">
@@ -10451,7 +10460,7 @@
       <c r="J66" s="39"/>
       <c r="K66" s="21"/>
     </row>
-    <row r="67" spans="1:11" ht="15">
+    <row r="67" spans="1:11">
       <c r="A67" s="18">
         <v>8</v>
       </c>
@@ -10495,9 +10504,9 @@
       <c r="J68" s="39"/>
       <c r="K68" s="21"/>
     </row>
-    <row r="69" spans="1:11" s="193" customFormat="1" ht="15" customHeight="1">
+    <row r="69" spans="1:11" s="156" customFormat="1" ht="15" customHeight="1">
       <c r="A69" s="18"/>
-      <c r="B69" s="189" t="s">
+      <c r="B69" s="152" t="s">
         <v>152</v>
       </c>
       <c r="C69" s="19">
@@ -10512,18 +10521,18 @@
         <v>0.53</v>
       </c>
       <c r="F69" s="21"/>
-      <c r="G69" s="191">
+      <c r="G69" s="154">
         <f>PRODUCT(C69:F69)</f>
         <v>3.7153306918622371</v>
       </c>
       <c r="H69" s="22"/>
       <c r="I69" s="23"/>
-      <c r="J69" s="192"/>
+      <c r="J69" s="155"/>
       <c r="K69" s="21"/>
     </row>
-    <row r="70" spans="1:11" s="193" customFormat="1" ht="15" customHeight="1">
+    <row r="70" spans="1:11" s="156" customFormat="1" ht="15" customHeight="1">
       <c r="A70" s="18"/>
-      <c r="B70" s="189" t="str">
+      <c r="B70" s="152" t="str">
         <f>B117</f>
         <v>-at entrance</v>
       </c>
@@ -10531,20 +10540,20 @@
         <f>C117</f>
         <v>1</v>
       </c>
-      <c r="D70" s="190">
+      <c r="D70" s="153">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E70" s="190">
+      <c r="E70" s="153">
         <v>0.9</v>
       </c>
-      <c r="F70" s="189"/>
-      <c r="G70" s="191">
+      <c r="F70" s="152"/>
+      <c r="G70" s="154">
         <f>PRODUCT(C70:F70)</f>
         <v>1.9800000000000002</v>
       </c>
       <c r="H70" s="22"/>
       <c r="I70" s="23"/>
-      <c r="J70" s="192"/>
+      <c r="J70" s="155"/>
       <c r="K70" s="21"/>
     </row>
     <row r="71" spans="1:11" ht="15" customHeight="1">
@@ -10779,7 +10788,7 @@
       </c>
       <c r="K80" s="21"/>
     </row>
-    <row r="81" spans="1:20" ht="15">
+    <row r="81" spans="1:20">
       <c r="A81" s="18"/>
       <c r="B81" s="88"/>
       <c r="C81" s="19"/>
@@ -10792,7 +10801,7 @@
       <c r="J81" s="39"/>
       <c r="K81" s="21"/>
     </row>
-    <row r="82" spans="1:20" ht="39">
+    <row r="82" spans="1:20" ht="39.75">
       <c r="A82" s="18">
         <v>10</v>
       </c>
@@ -10843,16 +10852,16 @@
       <c r="H83" s="38"/>
       <c r="I83" s="38"/>
       <c r="J83" s="38"/>
-      <c r="K83" s="60"/>
-      <c r="N83" s="166" t="s">
+      <c r="K83" s="222"/>
+      <c r="N83" s="196" t="s">
         <v>87</v>
       </c>
-      <c r="O83" s="166"/>
-      <c r="P83" s="166"/>
-      <c r="Q83" s="166"/>
-      <c r="R83" s="166"/>
-      <c r="S83" s="166"/>
-      <c r="T83" s="166"/>
+      <c r="O83" s="196"/>
+      <c r="P83" s="196"/>
+      <c r="Q83" s="196"/>
+      <c r="R83" s="196"/>
+      <c r="S83" s="196"/>
+      <c r="T83" s="196"/>
     </row>
     <row r="84" spans="1:20" ht="15" customHeight="1">
       <c r="A84" s="18"/>
@@ -10876,7 +10885,7 @@
       <c r="H84" s="38"/>
       <c r="I84" s="38"/>
       <c r="J84" s="38"/>
-      <c r="K84" s="60"/>
+      <c r="K84" s="222"/>
       <c r="N84" s="143"/>
       <c r="O84" s="143"/>
       <c r="P84" s="143"/>
@@ -11038,7 +11047,7 @@
         <v>3</v>
       </c>
       <c r="D91" s="20">
-        <f t="shared" ref="D91:D94" si="5">0.66-0.1</f>
+        <f t="shared" ref="D91" si="5">0.66-0.1</f>
         <v>0.56000000000000005</v>
       </c>
       <c r="E91" s="21">
@@ -11255,184 +11264,184 @@
       <c r="K99" s="21"/>
     </row>
     <row r="100" spans="1:22" ht="30">
-      <c r="A100" s="181">
+      <c r="A100" s="144">
         <v>12</v>
       </c>
-      <c r="B100" s="194" t="s">
+      <c r="B100" s="157" t="s">
         <v>100</v>
       </c>
-      <c r="C100" s="184"/>
-      <c r="D100" s="185"/>
-      <c r="E100" s="186"/>
-      <c r="F100" s="186"/>
-      <c r="G100" s="195"/>
-      <c r="H100" s="196"/>
-      <c r="I100" s="195"/>
-      <c r="J100" s="197"/>
+      <c r="C100" s="147"/>
+      <c r="D100" s="148"/>
+      <c r="E100" s="149"/>
+      <c r="F100" s="149"/>
+      <c r="G100" s="158"/>
+      <c r="H100" s="159"/>
+      <c r="I100" s="158"/>
+      <c r="J100" s="160"/>
       <c r="K100" s="21"/>
     </row>
     <row r="101" spans="1:22" ht="15" customHeight="1">
-      <c r="A101" s="181"/>
-      <c r="B101" s="183" t="s">
+      <c r="A101" s="144"/>
+      <c r="B101" s="146" t="s">
         <v>101</v>
       </c>
-      <c r="C101" s="198">
+      <c r="C101" s="161">
         <f>2*8</f>
         <v>16</v>
       </c>
-      <c r="D101" s="199">
+      <c r="D101" s="162">
         <v>0.66</v>
       </c>
-      <c r="E101" s="199"/>
-      <c r="F101" s="199">
+      <c r="E101" s="162"/>
+      <c r="F101" s="162">
         <v>0.1</v>
       </c>
-      <c r="G101" s="187">
+      <c r="G101" s="150">
         <f>PRODUCT(C101:F101)</f>
         <v>1.056</v>
       </c>
-      <c r="H101" s="200"/>
-      <c r="I101" s="200"/>
-      <c r="J101" s="200"/>
-      <c r="K101" s="60"/>
+      <c r="H101" s="163"/>
+      <c r="I101" s="163"/>
+      <c r="J101" s="163"/>
+      <c r="K101" s="222"/>
     </row>
     <row r="102" spans="1:22" ht="15" customHeight="1">
-      <c r="A102" s="181"/>
-      <c r="B102" s="183"/>
-      <c r="C102" s="198">
+      <c r="A102" s="144"/>
+      <c r="B102" s="146"/>
+      <c r="C102" s="161">
         <f>2*8</f>
         <v>16</v>
       </c>
-      <c r="D102" s="199">
+      <c r="D102" s="162">
         <v>0.92</v>
       </c>
-      <c r="E102" s="199"/>
-      <c r="F102" s="199">
+      <c r="E102" s="162"/>
+      <c r="F102" s="162">
         <v>0.1</v>
       </c>
-      <c r="G102" s="187">
+      <c r="G102" s="150">
         <f t="shared" ref="G102:G108" si="9">PRODUCT(C102:F102)</f>
         <v>1.4720000000000002</v>
       </c>
-      <c r="H102" s="200"/>
-      <c r="I102" s="200"/>
-      <c r="J102" s="200"/>
-      <c r="K102" s="60"/>
+      <c r="H102" s="163"/>
+      <c r="I102" s="163"/>
+      <c r="J102" s="163"/>
+      <c r="K102" s="222"/>
     </row>
     <row r="103" spans="1:22" ht="15" customHeight="1">
-      <c r="A103" s="181"/>
-      <c r="B103" s="183"/>
-      <c r="C103" s="198">
+      <c r="A103" s="144"/>
+      <c r="B103" s="146"/>
+      <c r="C103" s="161">
         <f>2*1</f>
         <v>2</v>
       </c>
-      <c r="D103" s="199">
+      <c r="D103" s="162">
         <v>0.66</v>
       </c>
-      <c r="E103" s="199"/>
-      <c r="F103" s="199">
+      <c r="E103" s="162"/>
+      <c r="F103" s="162">
         <v>0.1</v>
       </c>
-      <c r="G103" s="187">
+      <c r="G103" s="150">
         <f t="shared" si="9"/>
         <v>0.13200000000000001</v>
       </c>
-      <c r="H103" s="200"/>
-      <c r="I103" s="200"/>
-      <c r="J103" s="200"/>
-      <c r="K103" s="60"/>
+      <c r="H103" s="163"/>
+      <c r="I103" s="163"/>
+      <c r="J103" s="163"/>
+      <c r="K103" s="222"/>
     </row>
     <row r="104" spans="1:22" ht="15" customHeight="1">
-      <c r="A104" s="181"/>
-      <c r="B104" s="183"/>
-      <c r="C104" s="198">
+      <c r="A104" s="144"/>
+      <c r="B104" s="146"/>
+      <c r="C104" s="161">
         <f>2*1</f>
         <v>2</v>
       </c>
-      <c r="D104" s="199">
+      <c r="D104" s="162">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E104" s="199"/>
-      <c r="F104" s="199">
+      <c r="E104" s="162"/>
+      <c r="F104" s="162">
         <v>0.1</v>
       </c>
-      <c r="G104" s="187">
+      <c r="G104" s="150">
         <f t="shared" si="9"/>
         <v>0.11399999999999999</v>
       </c>
-      <c r="H104" s="200"/>
-      <c r="I104" s="200"/>
-      <c r="J104" s="200"/>
-      <c r="K104" s="60"/>
+      <c r="H104" s="163"/>
+      <c r="I104" s="163"/>
+      <c r="J104" s="163"/>
+      <c r="K104" s="222"/>
     </row>
     <row r="105" spans="1:22" ht="15" customHeight="1">
-      <c r="A105" s="181"/>
-      <c r="B105" s="183"/>
-      <c r="C105" s="198">
+      <c r="A105" s="144"/>
+      <c r="B105" s="146"/>
+      <c r="C105" s="161">
         <f t="shared" ref="C105:C108" si="10">2*1</f>
         <v>2</v>
       </c>
-      <c r="D105" s="199">
+      <c r="D105" s="162">
         <v>1.65</v>
       </c>
-      <c r="E105" s="199"/>
-      <c r="F105" s="199">
+      <c r="E105" s="162"/>
+      <c r="F105" s="162">
         <v>0.1</v>
       </c>
-      <c r="G105" s="187">
+      <c r="G105" s="150">
         <f t="shared" si="9"/>
         <v>0.33</v>
       </c>
-      <c r="H105" s="200"/>
-      <c r="I105" s="200"/>
-      <c r="J105" s="200"/>
-      <c r="K105" s="60"/>
+      <c r="H105" s="163"/>
+      <c r="I105" s="163"/>
+      <c r="J105" s="163"/>
+      <c r="K105" s="222"/>
     </row>
     <row r="106" spans="1:22" ht="15" customHeight="1">
-      <c r="A106" s="181"/>
-      <c r="B106" s="183"/>
-      <c r="C106" s="198">
+      <c r="A106" s="144"/>
+      <c r="B106" s="146"/>
+      <c r="C106" s="161">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="D106" s="199">
+      <c r="D106" s="162">
         <v>0.84</v>
       </c>
-      <c r="E106" s="199"/>
-      <c r="F106" s="199">
+      <c r="E106" s="162"/>
+      <c r="F106" s="162">
         <v>0.1</v>
       </c>
-      <c r="G106" s="187">
+      <c r="G106" s="150">
         <f t="shared" si="9"/>
         <v>0.16800000000000001</v>
       </c>
-      <c r="H106" s="200"/>
-      <c r="I106" s="200"/>
-      <c r="J106" s="200"/>
-      <c r="K106" s="60"/>
+      <c r="H106" s="163"/>
+      <c r="I106" s="163"/>
+      <c r="J106" s="163"/>
+      <c r="K106" s="222"/>
     </row>
     <row r="107" spans="1:22" ht="15" customHeight="1">
-      <c r="A107" s="181"/>
-      <c r="B107" s="183"/>
-      <c r="C107" s="198">
+      <c r="A107" s="144"/>
+      <c r="B107" s="146"/>
+      <c r="C107" s="161">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="D107" s="199">
+      <c r="D107" s="162">
         <v>0.92</v>
       </c>
-      <c r="E107" s="199"/>
-      <c r="F107" s="199">
+      <c r="E107" s="162"/>
+      <c r="F107" s="162">
         <v>0.1</v>
       </c>
-      <c r="G107" s="187">
+      <c r="G107" s="150">
         <f t="shared" si="9"/>
         <v>0.18400000000000002</v>
       </c>
-      <c r="H107" s="200"/>
-      <c r="I107" s="200"/>
-      <c r="J107" s="200"/>
-      <c r="K107" s="60"/>
+      <c r="H107" s="163"/>
+      <c r="I107" s="163"/>
+      <c r="J107" s="163"/>
+      <c r="K107" s="222"/>
       <c r="M107" s="127"/>
       <c r="N107" s="1"/>
       <c r="O107" s="1"/>
@@ -11445,27 +11454,27 @@
       <c r="V107" s="1"/>
     </row>
     <row r="108" spans="1:22" ht="15" customHeight="1">
-      <c r="A108" s="181"/>
-      <c r="B108" s="183"/>
-      <c r="C108" s="198">
+      <c r="A108" s="144"/>
+      <c r="B108" s="146"/>
+      <c r="C108" s="161">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="D108" s="199">
+      <c r="D108" s="162">
         <v>0.8</v>
       </c>
-      <c r="E108" s="199"/>
-      <c r="F108" s="199">
+      <c r="E108" s="162"/>
+      <c r="F108" s="162">
         <v>0.1</v>
       </c>
-      <c r="G108" s="187">
+      <c r="G108" s="150">
         <f t="shared" si="9"/>
         <v>0.16000000000000003</v>
       </c>
-      <c r="H108" s="200"/>
-      <c r="I108" s="200"/>
-      <c r="J108" s="200"/>
-      <c r="K108" s="60"/>
+      <c r="H108" s="163"/>
+      <c r="I108" s="163"/>
+      <c r="J108" s="163"/>
+      <c r="K108" s="222"/>
       <c r="M108" s="127"/>
       <c r="N108" s="1"/>
       <c r="O108" s="1"/>
@@ -11478,26 +11487,26 @@
       <c r="V108" s="1"/>
     </row>
     <row r="109" spans="1:22" ht="15" customHeight="1">
-      <c r="A109" s="181"/>
-      <c r="B109" s="183" t="s">
+      <c r="A109" s="144"/>
+      <c r="B109" s="146" t="s">
         <v>41</v>
       </c>
-      <c r="C109" s="198"/>
-      <c r="D109" s="199"/>
-      <c r="E109" s="199"/>
-      <c r="F109" s="199"/>
-      <c r="G109" s="201">
+      <c r="C109" s="161"/>
+      <c r="D109" s="162"/>
+      <c r="E109" s="162"/>
+      <c r="F109" s="162"/>
+      <c r="G109" s="164">
         <f>SUM(G101:G108)</f>
         <v>3.616000000000001</v>
       </c>
-      <c r="H109" s="200" t="s">
+      <c r="H109" s="163" t="s">
         <v>43</v>
       </c>
-      <c r="I109" s="195">
+      <c r="I109" s="158">
         <f>81404.27/100</f>
         <v>814.04270000000008</v>
       </c>
-      <c r="J109" s="202">
+      <c r="J109" s="165">
         <f>G109*I109</f>
         <v>2943.578403200001</v>
       </c>
@@ -11514,18 +11523,18 @@
       <c r="V109" s="1"/>
     </row>
     <row r="110" spans="1:22" ht="15" customHeight="1">
-      <c r="A110" s="181"/>
-      <c r="B110" s="183" t="s">
+      <c r="A110" s="144"/>
+      <c r="B110" s="146" t="s">
         <v>40</v>
       </c>
-      <c r="C110" s="198"/>
-      <c r="D110" s="199"/>
-      <c r="E110" s="199"/>
-      <c r="F110" s="199"/>
-      <c r="G110" s="187"/>
-      <c r="H110" s="200"/>
-      <c r="I110" s="200"/>
-      <c r="J110" s="202">
+      <c r="C110" s="161"/>
+      <c r="D110" s="162"/>
+      <c r="E110" s="162"/>
+      <c r="F110" s="162"/>
+      <c r="G110" s="150"/>
+      <c r="H110" s="163"/>
+      <c r="I110" s="163"/>
+      <c r="J110" s="165">
         <f>0.13*G109*36690.27/100</f>
         <v>172.47362121600003</v>
       </c>
@@ -11616,7 +11625,7 @@
       <c r="H113" s="38"/>
       <c r="I113" s="38"/>
       <c r="J113" s="38"/>
-      <c r="K113" s="60"/>
+      <c r="K113" s="222"/>
       <c r="M113" s="127"/>
       <c r="N113" s="1"/>
       <c r="O113" s="1"/>
@@ -11651,7 +11660,7 @@
       <c r="H114" s="38"/>
       <c r="I114" s="38"/>
       <c r="J114" s="38"/>
-      <c r="K114" s="60"/>
+      <c r="K114" s="222"/>
       <c r="M114" s="127">
         <f>E113*8+E114+D115+D116</f>
         <v>10.5</v>
@@ -11689,7 +11698,7 @@
       <c r="H115" s="38"/>
       <c r="I115" s="38"/>
       <c r="J115" s="38"/>
-      <c r="K115" s="60"/>
+      <c r="K115" s="222"/>
       <c r="M115" s="127"/>
       <c r="N115" s="1"/>
       <c r="O115" s="1"/>
@@ -11724,7 +11733,7 @@
       <c r="H116" s="38"/>
       <c r="I116" s="38"/>
       <c r="J116" s="38"/>
-      <c r="K116" s="60"/>
+      <c r="K116" s="222"/>
       <c r="M116" s="127"/>
       <c r="N116" s="1"/>
       <c r="O116" s="1"/>
@@ -11762,7 +11771,7 @@
       <c r="H117" s="38"/>
       <c r="I117" s="38"/>
       <c r="J117" s="38"/>
-      <c r="K117" s="60"/>
+      <c r="K117" s="222"/>
     </row>
     <row r="118" spans="1:22" ht="15" customHeight="1">
       <c r="A118" s="18"/>
@@ -11830,7 +11839,7 @@
       <c r="U120" s="1"/>
       <c r="V120" s="1"/>
     </row>
-    <row r="121" spans="1:22" ht="30.6">
+    <row r="121" spans="1:22" ht="30.75">
       <c r="A121" s="18">
         <v>14</v>
       </c>
@@ -11982,7 +11991,7 @@
       <c r="U124" s="1"/>
       <c r="V124" s="1"/>
     </row>
-    <row r="125" spans="1:22" s="1" customFormat="1" ht="27.6">
+    <row r="125" spans="1:22" s="1" customFormat="1" ht="30">
       <c r="A125" s="120"/>
       <c r="B125" s="125" t="s">
         <v>125</v>
@@ -12061,7 +12070,7 @@
     </row>
     <row r="128" spans="1:22" s="1" customFormat="1">
       <c r="A128" s="120"/>
-      <c r="B128" s="221" t="s">
+      <c r="B128" s="184" t="s">
         <v>157</v>
       </c>
       <c r="C128" s="122">
@@ -12088,7 +12097,7 @@
     </row>
     <row r="129" spans="1:22" s="1" customFormat="1">
       <c r="A129" s="120"/>
-      <c r="B129" s="220"/>
+      <c r="B129" s="183"/>
       <c r="C129" s="122">
         <v>4</v>
       </c>
@@ -12111,7 +12120,7 @@
       <c r="J129" s="123"/>
       <c r="K129" s="121"/>
     </row>
-    <row r="130" spans="1:22" s="1" customFormat="1" ht="41.4">
+    <row r="130" spans="1:22" s="1" customFormat="1" ht="45">
       <c r="A130" s="120"/>
       <c r="B130" s="125" t="s">
         <v>126</v>
@@ -12217,7 +12226,7 @@
       <c r="J133" s="123"/>
       <c r="K133" s="121"/>
     </row>
-    <row r="134" spans="1:22" s="1" customFormat="1" ht="27.6">
+    <row r="134" spans="1:22" s="1" customFormat="1" ht="30">
       <c r="A134" s="120"/>
       <c r="B134" s="125" t="s">
         <v>132</v>
@@ -12421,7 +12430,7 @@
       <c r="H141" s="38"/>
       <c r="I141" s="38"/>
       <c r="J141" s="38"/>
-      <c r="K141" s="60"/>
+      <c r="K141" s="222"/>
       <c r="N141">
         <f>5.84+1.76</f>
         <v>7.6</v>
@@ -12449,7 +12458,7 @@
       <c r="H142" s="38"/>
       <c r="I142" s="38"/>
       <c r="J142" s="38"/>
-      <c r="K142" s="60"/>
+      <c r="K142" s="222"/>
     </row>
     <row r="143" spans="1:22" ht="15" customHeight="1">
       <c r="A143" s="18"/>
@@ -12473,7 +12482,7 @@
       <c r="H143" s="38"/>
       <c r="I143" s="38"/>
       <c r="J143" s="38"/>
-      <c r="K143" s="60"/>
+      <c r="K143" s="222"/>
     </row>
     <row r="144" spans="1:22" ht="15" customHeight="1">
       <c r="A144" s="18"/>
@@ -12497,7 +12506,7 @@
       <c r="H144" s="38"/>
       <c r="I144" s="38"/>
       <c r="J144" s="38"/>
-      <c r="K144" s="60"/>
+      <c r="K144" s="222"/>
     </row>
     <row r="145" spans="1:11" ht="15" customHeight="1">
       <c r="A145" s="18"/>
@@ -12521,7 +12530,7 @@
       <c r="H145" s="38"/>
       <c r="I145" s="38"/>
       <c r="J145" s="38"/>
-      <c r="K145" s="60"/>
+      <c r="K145" s="222"/>
     </row>
     <row r="146" spans="1:11" ht="15" customHeight="1">
       <c r="A146" s="18"/>
@@ -12545,7 +12554,7 @@
       <c r="H146" s="38"/>
       <c r="I146" s="38"/>
       <c r="J146" s="38"/>
-      <c r="K146" s="60"/>
+      <c r="K146" s="222"/>
     </row>
     <row r="147" spans="1:11" ht="15" customHeight="1">
       <c r="A147" s="18"/>
@@ -12569,7 +12578,7 @@
       <c r="H147" s="38"/>
       <c r="I147" s="38"/>
       <c r="J147" s="38"/>
-      <c r="K147" s="60"/>
+      <c r="K147" s="222"/>
     </row>
     <row r="148" spans="1:11" ht="15" customHeight="1">
       <c r="A148" s="18"/>
@@ -12593,7 +12602,7 @@
       <c r="H148" s="38"/>
       <c r="I148" s="38"/>
       <c r="J148" s="38"/>
-      <c r="K148" s="60"/>
+      <c r="K148" s="222"/>
     </row>
     <row r="149" spans="1:11" ht="15" customHeight="1">
       <c r="A149" s="18"/>
@@ -12617,7 +12626,7 @@
       <c r="H149" s="38"/>
       <c r="I149" s="38"/>
       <c r="J149" s="38"/>
-      <c r="K149" s="60"/>
+      <c r="K149" s="222"/>
     </row>
     <row r="150" spans="1:11" ht="15" customHeight="1">
       <c r="A150" s="18"/>
@@ -12641,7 +12650,7 @@
       <c r="H150" s="38"/>
       <c r="I150" s="38"/>
       <c r="J150" s="38"/>
-      <c r="K150" s="60"/>
+      <c r="K150" s="222"/>
     </row>
     <row r="151" spans="1:11" ht="15" customHeight="1">
       <c r="A151" s="18"/>
@@ -12665,7 +12674,7 @@
       <c r="H151" s="38"/>
       <c r="I151" s="38"/>
       <c r="J151" s="38"/>
-      <c r="K151" s="60"/>
+      <c r="K151" s="222"/>
     </row>
     <row r="152" spans="1:11" ht="15" customHeight="1">
       <c r="A152" s="18"/>
@@ -12689,7 +12698,7 @@
       <c r="H152" s="38"/>
       <c r="I152" s="38"/>
       <c r="J152" s="38"/>
-      <c r="K152" s="60"/>
+      <c r="K152" s="222"/>
     </row>
     <row r="153" spans="1:11" ht="15" customHeight="1">
       <c r="A153" s="18"/>
@@ -12712,7 +12721,7 @@
       <c r="H153" s="38"/>
       <c r="I153" s="38"/>
       <c r="J153" s="38"/>
-      <c r="K153" s="60"/>
+      <c r="K153" s="222"/>
     </row>
     <row r="154" spans="1:11" ht="15" customHeight="1">
       <c r="A154" s="18"/>
@@ -12738,7 +12747,7 @@
       <c r="H154" s="38"/>
       <c r="I154" s="38"/>
       <c r="J154" s="38"/>
-      <c r="K154" s="60"/>
+      <c r="K154" s="222"/>
     </row>
     <row r="155" spans="1:11" ht="15" customHeight="1">
       <c r="A155" s="18"/>
@@ -12763,13 +12772,13 @@
       <c r="H155" s="38"/>
       <c r="I155" s="38"/>
       <c r="J155" s="38"/>
-      <c r="K155" s="60"/>
+      <c r="K155" s="222"/>
     </row>
     <row r="156" spans="1:11" ht="15" customHeight="1">
       <c r="A156" s="18"/>
       <c r="B156" s="35"/>
       <c r="C156" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D156" s="36">
         <f>14/3.281</f>
@@ -12782,18 +12791,18 @@
       </c>
       <c r="G156" s="37">
         <f t="shared" si="27"/>
-        <v>14.507772020725389</v>
+        <v>7.2538860103626943</v>
       </c>
       <c r="H156" s="38"/>
       <c r="I156" s="38"/>
       <c r="J156" s="38"/>
-      <c r="K156" s="60"/>
+      <c r="K156" s="222"/>
     </row>
     <row r="157" spans="1:11" ht="15" customHeight="1">
       <c r="A157" s="18"/>
       <c r="B157" s="35"/>
       <c r="C157" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D157" s="36">
         <f>(22.5/3.281)</f>
@@ -12806,18 +12815,18 @@
       </c>
       <c r="G157" s="37">
         <f t="shared" si="27"/>
-        <v>17.829929899420907</v>
+        <v>8.9149649497104537</v>
       </c>
       <c r="H157" s="38"/>
       <c r="I157" s="38"/>
       <c r="J157" s="38"/>
-      <c r="K157" s="60"/>
+      <c r="K157" s="222"/>
     </row>
     <row r="158" spans="1:11" ht="15" customHeight="1">
       <c r="A158" s="18"/>
       <c r="B158" s="35"/>
       <c r="C158" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D158" s="36">
         <f>(19/3.281)</f>
@@ -12830,18 +12839,18 @@
       </c>
       <c r="G158" s="37">
         <f t="shared" si="27"/>
-        <v>13.377019201462968</v>
+        <v>6.6885096007314839</v>
       </c>
       <c r="H158" s="38"/>
       <c r="I158" s="38"/>
       <c r="J158" s="38"/>
-      <c r="K158" s="60"/>
+      <c r="K158" s="222"/>
     </row>
     <row r="159" spans="1:11" ht="15" customHeight="1">
       <c r="A159" s="18"/>
       <c r="B159" s="35"/>
       <c r="C159" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D159" s="36">
         <f>34.5/3.281</f>
@@ -12854,18 +12863,18 @@
       </c>
       <c r="G159" s="37">
         <f t="shared" si="27"/>
-        <v>15.24687595245352</v>
+        <v>7.6234379762267599</v>
       </c>
       <c r="H159" s="38"/>
       <c r="I159" s="38"/>
       <c r="J159" s="38"/>
-      <c r="K159" s="60"/>
+      <c r="K159" s="222"/>
     </row>
     <row r="160" spans="1:11" ht="15" customHeight="1">
       <c r="A160" s="18"/>
       <c r="B160" s="35"/>
       <c r="C160" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D160" s="36">
         <f>34.75/3.281</f>
@@ -12877,18 +12886,18 @@
       </c>
       <c r="G160" s="37">
         <f t="shared" si="27"/>
-        <v>27.537336177994515</v>
+        <v>13.768668088997257</v>
       </c>
       <c r="H160" s="38"/>
       <c r="I160" s="38"/>
       <c r="J160" s="38"/>
-      <c r="K160" s="60"/>
+      <c r="K160" s="222"/>
     </row>
     <row r="161" spans="1:22" ht="15" customHeight="1">
       <c r="A161" s="18"/>
       <c r="B161" s="35"/>
       <c r="C161" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D161" s="36">
         <f>3.12-0.3</f>
@@ -12900,18 +12909,18 @@
       </c>
       <c r="G161" s="37">
         <f t="shared" si="27"/>
-        <v>10.716000000000001</v>
+        <v>5.3580000000000005</v>
       </c>
       <c r="H161" s="38"/>
       <c r="I161" s="38"/>
       <c r="J161" s="38"/>
-      <c r="K161" s="60"/>
+      <c r="K161" s="222"/>
     </row>
     <row r="162" spans="1:22" ht="15" customHeight="1">
       <c r="A162" s="18"/>
       <c r="B162" s="35"/>
       <c r="C162" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D162" s="36">
         <f>22.583/3.281</f>
@@ -12924,18 +12933,18 @@
       </c>
       <c r="G162" s="37">
         <f t="shared" si="27"/>
-        <v>7.8465772630295634</v>
+        <v>3.9232886315147817</v>
       </c>
       <c r="H162" s="38"/>
       <c r="I162" s="38"/>
       <c r="J162" s="38"/>
-      <c r="K162" s="60"/>
+      <c r="K162" s="222"/>
     </row>
     <row r="163" spans="1:22" ht="15" customHeight="1">
       <c r="A163" s="18"/>
       <c r="B163" s="35"/>
       <c r="C163" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D163" s="36">
         <f>13/3.281</f>
@@ -12948,18 +12957,18 @@
       </c>
       <c r="G163" s="37">
         <f t="shared" si="27"/>
-        <v>4.5169155745199641</v>
+        <v>2.258457787259982</v>
       </c>
       <c r="H163" s="38"/>
       <c r="I163" s="38"/>
       <c r="J163" s="38"/>
-      <c r="K163" s="60"/>
+      <c r="K163" s="222"/>
     </row>
     <row r="164" spans="1:22" ht="15" customHeight="1">
       <c r="A164" s="18"/>
       <c r="B164" s="35"/>
       <c r="C164" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D164" s="36">
         <f>22.583/3.281</f>
@@ -12971,18 +12980,18 @@
       </c>
       <c r="G164" s="37">
         <f t="shared" si="27"/>
-        <v>4.1297775068576641</v>
+        <v>2.064888753428832</v>
       </c>
       <c r="H164" s="38"/>
       <c r="I164" s="38"/>
       <c r="J164" s="38"/>
-      <c r="K164" s="60"/>
+      <c r="K164" s="222"/>
     </row>
     <row r="165" spans="1:22" ht="15" customHeight="1">
       <c r="A165" s="18"/>
       <c r="B165" s="35"/>
       <c r="C165" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D165" s="36">
         <v>2.1</v>
@@ -12993,18 +13002,18 @@
       </c>
       <c r="G165" s="37">
         <f t="shared" si="27"/>
-        <v>2.4359999999999999</v>
+        <v>1.218</v>
       </c>
       <c r="H165" s="38"/>
       <c r="I165" s="38"/>
       <c r="J165" s="38"/>
-      <c r="K165" s="60"/>
+      <c r="K165" s="222"/>
     </row>
     <row r="166" spans="1:22" ht="15" customHeight="1">
       <c r="A166" s="18"/>
       <c r="B166" s="35"/>
       <c r="C166" s="34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D166" s="36">
         <v>1.5</v>
@@ -13015,12 +13024,12 @@
       </c>
       <c r="G166" s="37">
         <f t="shared" si="27"/>
-        <v>1.17</v>
+        <v>0.58499999999999996</v>
       </c>
       <c r="H166" s="38"/>
       <c r="I166" s="38"/>
       <c r="J166" s="38"/>
-      <c r="K166" s="60"/>
+      <c r="K166" s="222"/>
     </row>
     <row r="167" spans="1:22" ht="15" customHeight="1">
       <c r="A167" s="18"/>
@@ -13043,7 +13052,7 @@
       <c r="H167" s="38"/>
       <c r="I167" s="38"/>
       <c r="J167" s="38"/>
-      <c r="K167" s="60"/>
+      <c r="K167" s="222"/>
     </row>
     <row r="168" spans="1:22" ht="15" customHeight="1">
       <c r="A168" s="18"/>
@@ -13067,7 +13076,7 @@
       <c r="H168" s="38"/>
       <c r="I168" s="38"/>
       <c r="J168" s="38"/>
-      <c r="K168" s="60"/>
+      <c r="K168" s="222"/>
     </row>
     <row r="169" spans="1:22" ht="15" customHeight="1">
       <c r="A169" s="18"/>
@@ -13090,7 +13099,7 @@
       <c r="H169" s="38"/>
       <c r="I169" s="38"/>
       <c r="J169" s="38"/>
-      <c r="K169" s="60"/>
+      <c r="K169" s="222"/>
     </row>
     <row r="170" spans="1:22" ht="15" customHeight="1">
       <c r="A170" s="18"/>
@@ -13103,7 +13112,7 @@
       <c r="F170" s="36"/>
       <c r="G170" s="37">
         <f>SUM(G141:G169)</f>
-        <v>187.88588744285281</v>
+        <v>128.22878564462053</v>
       </c>
       <c r="H170" s="38" t="s">
         <v>43</v>
@@ -13113,11 +13122,11 @@
       </c>
       <c r="J170" s="38">
         <f>G170*I170</f>
-        <v>76255.366277556241</v>
-      </c>
-      <c r="K170" s="60"/>
-    </row>
-    <row r="171" spans="1:22" s="1" customFormat="1" ht="17.399999999999999">
+        <v>52042.934941725689</v>
+      </c>
+      <c r="K170" s="222"/>
+    </row>
+    <row r="171" spans="1:22" s="1" customFormat="1" ht="18">
       <c r="A171" s="18"/>
       <c r="B171" s="125" t="s">
         <v>130</v>
@@ -13131,22 +13140,22 @@
       <c r="I171" s="23"/>
       <c r="J171" s="123">
         <f>0.13*G170*11166.2/100</f>
-        <v>2727.3628152736983</v>
+        <v>1861.3767461444502</v>
       </c>
       <c r="K171" s="21"/>
-      <c r="N171" s="180" t="s">
+      <c r="N171" s="186" t="s">
         <v>143</v>
       </c>
-      <c r="O171" s="180"/>
-      <c r="P171" s="180"/>
-      <c r="Q171" s="180"/>
-      <c r="R171" s="180"/>
-      <c r="S171" s="180"/>
-      <c r="T171" s="180"/>
+      <c r="O171" s="186"/>
+      <c r="P171" s="186"/>
+      <c r="Q171" s="186"/>
+      <c r="R171" s="186"/>
+      <c r="S171" s="186"/>
+      <c r="T171" s="186"/>
       <c r="U171"/>
       <c r="V171"/>
     </row>
-    <row r="172" spans="1:22" s="1" customFormat="1" ht="17.399999999999999">
+    <row r="172" spans="1:22" s="1" customFormat="1" ht="18">
       <c r="A172" s="18"/>
       <c r="B172" s="125"/>
       <c r="C172" s="19"/>
@@ -13158,19 +13167,19 @@
       <c r="I172" s="23"/>
       <c r="J172" s="123"/>
       <c r="K172" s="21"/>
-      <c r="N172" s="180" t="s">
+      <c r="N172" s="186" t="s">
         <v>144</v>
       </c>
-      <c r="O172" s="180"/>
-      <c r="P172" s="180"/>
-      <c r="Q172" s="180"/>
-      <c r="R172" s="180"/>
-      <c r="S172" s="180"/>
-      <c r="T172" s="180"/>
+      <c r="O172" s="186"/>
+      <c r="P172" s="186"/>
+      <c r="Q172" s="186"/>
+      <c r="R172" s="186"/>
+      <c r="S172" s="186"/>
+      <c r="T172" s="186"/>
       <c r="U172"/>
       <c r="V172"/>
     </row>
-    <row r="173" spans="1:22" ht="30.6">
+    <row r="173" spans="1:22" ht="30.75">
       <c r="A173" s="18">
         <v>16</v>
       </c>
@@ -13200,7 +13209,7 @@
       <c r="F174" s="21"/>
       <c r="G174" s="37">
         <f>G170-G155</f>
-        <v>183.2658874428528</v>
+        <v>123.60878564462053</v>
       </c>
       <c r="H174" s="22"/>
       <c r="I174" s="23"/>
@@ -13263,7 +13272,7 @@
       <c r="J177" s="39"/>
       <c r="K177" s="21"/>
     </row>
-    <row r="178" spans="1:22" s="1" customFormat="1" ht="46.2">
+    <row r="178" spans="1:22" s="1" customFormat="1" ht="48">
       <c r="A178" s="18">
         <v>17</v>
       </c>
@@ -13272,6 +13281,8 @@
       </c>
       <c r="C178" s="140"/>
       <c r="D178" s="20"/>
+      <c r="E178" s="121"/>
+      <c r="F178" s="121"/>
       <c r="G178" s="123"/>
       <c r="H178" s="22"/>
       <c r="I178" s="23"/>
@@ -13423,365 +13434,365 @@
       <c r="J184" s="39"/>
       <c r="K184" s="21"/>
     </row>
-    <row r="185" spans="1:22" s="210" customFormat="1" ht="17.399999999999999">
-      <c r="A185" s="203">
+    <row r="185" spans="1:22" s="173" customFormat="1" ht="18">
+      <c r="A185" s="166">
         <v>18</v>
       </c>
-      <c r="B185" s="204" t="s">
+      <c r="B185" s="167" t="s">
         <v>139</v>
       </c>
-      <c r="C185" s="205"/>
-      <c r="D185" s="206"/>
-      <c r="E185" s="207"/>
-      <c r="F185" s="206" t="s">
+      <c r="C185" s="168"/>
+      <c r="D185" s="169"/>
+      <c r="E185" s="170"/>
+      <c r="F185" s="169" t="s">
         <v>163</v>
       </c>
-      <c r="G185" s="206"/>
-      <c r="H185" s="206"/>
-      <c r="I185" s="206"/>
-      <c r="J185" s="208"/>
-      <c r="K185" s="209"/>
-      <c r="M185" s="211"/>
-      <c r="N185" s="211"/>
-      <c r="O185" s="211"/>
-      <c r="P185" s="211"/>
-      <c r="Q185" s="211"/>
-      <c r="R185" s="211"/>
-      <c r="S185" s="211"/>
-      <c r="T185" s="211"/>
-      <c r="U185" s="211"/>
-      <c r="V185" s="211"/>
-    </row>
-    <row r="186" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A186" s="181"/>
-      <c r="B186" s="183" t="s">
+      <c r="G185" s="169"/>
+      <c r="H185" s="169"/>
+      <c r="I185" s="169"/>
+      <c r="J185" s="171"/>
+      <c r="K185" s="172"/>
+      <c r="M185" s="174"/>
+      <c r="N185" s="174"/>
+      <c r="O185" s="174"/>
+      <c r="P185" s="174"/>
+      <c r="Q185" s="174"/>
+      <c r="R185" s="174"/>
+      <c r="S185" s="174"/>
+      <c r="T185" s="174"/>
+      <c r="U185" s="174"/>
+      <c r="V185" s="174"/>
+    </row>
+    <row r="186" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A186" s="144"/>
+      <c r="B186" s="146" t="s">
         <v>140</v>
       </c>
-      <c r="C186" s="198">
+      <c r="C186" s="161">
         <v>1</v>
       </c>
-      <c r="D186" s="199"/>
-      <c r="E186" s="212"/>
-      <c r="F186" s="213">
+      <c r="D186" s="162"/>
+      <c r="E186" s="175"/>
+      <c r="F186" s="176">
         <f>CONVERT(48.3735,"ft2","m2")</f>
         <v>4.49404520544</v>
       </c>
-      <c r="G186" s="214">
+      <c r="G186" s="177">
         <f>PRODUCT(C186:F186)</f>
         <v>4.49404520544</v>
       </c>
-      <c r="H186" s="200"/>
-      <c r="I186" s="200"/>
-      <c r="J186" s="200"/>
-      <c r="K186" s="186"/>
-    </row>
-    <row r="187" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A187" s="181"/>
-      <c r="B187" s="183"/>
-      <c r="C187" s="198">
+      <c r="H186" s="163"/>
+      <c r="I186" s="163"/>
+      <c r="J186" s="163"/>
+      <c r="K186" s="149"/>
+    </row>
+    <row r="187" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A187" s="144"/>
+      <c r="B187" s="146"/>
+      <c r="C187" s="161">
         <v>1</v>
       </c>
-      <c r="D187" s="199"/>
-      <c r="E187" s="212"/>
-      <c r="F187" s="213">
+      <c r="D187" s="162"/>
+      <c r="E187" s="175"/>
+      <c r="F187" s="176">
         <f>CONVERT(224.2762,"ft2","m2")</f>
         <v>20.835940779647999</v>
       </c>
-      <c r="G187" s="214">
+      <c r="G187" s="177">
         <f>PRODUCT(C187:F187)</f>
         <v>20.835940779647999</v>
       </c>
-      <c r="H187" s="200"/>
-      <c r="I187" s="200"/>
-      <c r="J187" s="200"/>
-      <c r="K187" s="186"/>
-    </row>
-    <row r="188" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A188" s="181"/>
-      <c r="B188" s="183"/>
-      <c r="C188" s="198">
+      <c r="H187" s="163"/>
+      <c r="I187" s="163"/>
+      <c r="J187" s="163"/>
+      <c r="K187" s="149"/>
+    </row>
+    <row r="188" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A188" s="144"/>
+      <c r="B188" s="146"/>
+      <c r="C188" s="161">
         <v>1</v>
       </c>
-      <c r="D188" s="199">
+      <c r="D188" s="162">
         <f>(4.1+4.4)/2</f>
         <v>4.25</v>
       </c>
-      <c r="E188" s="199">
+      <c r="E188" s="162">
         <f>2.6</f>
         <v>2.6</v>
       </c>
-      <c r="F188" s="199"/>
-      <c r="G188" s="214">
+      <c r="F188" s="162"/>
+      <c r="G188" s="177">
         <f t="shared" ref="G188:G190" si="29">PRODUCT(C188:F188)</f>
         <v>11.05</v>
       </c>
-      <c r="H188" s="200"/>
-      <c r="I188" s="200"/>
-      <c r="J188" s="200"/>
-      <c r="K188" s="186"/>
-      <c r="M188" s="215"/>
-      <c r="N188" s="215"/>
-      <c r="O188" s="215"/>
-      <c r="P188" s="215"/>
-      <c r="Q188" s="215"/>
-      <c r="R188" s="215"/>
-      <c r="S188" s="215"/>
-      <c r="T188" s="215"/>
-      <c r="U188" s="215"/>
-      <c r="V188" s="215"/>
-    </row>
-    <row r="189" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A189" s="181"/>
-      <c r="B189" s="183"/>
-      <c r="C189" s="198">
+      <c r="H188" s="163"/>
+      <c r="I188" s="163"/>
+      <c r="J188" s="163"/>
+      <c r="K188" s="149"/>
+      <c r="M188" s="178"/>
+      <c r="N188" s="178"/>
+      <c r="O188" s="178"/>
+      <c r="P188" s="178"/>
+      <c r="Q188" s="178"/>
+      <c r="R188" s="178"/>
+      <c r="S188" s="178"/>
+      <c r="T188" s="178"/>
+      <c r="U188" s="178"/>
+      <c r="V188" s="178"/>
+    </row>
+    <row r="189" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A189" s="144"/>
+      <c r="B189" s="146"/>
+      <c r="C189" s="161">
         <v>1</v>
       </c>
-      <c r="D189" s="199">
+      <c r="D189" s="162">
         <v>7</v>
       </c>
-      <c r="E189" s="199">
+      <c r="E189" s="162">
         <f>((2.5+4.75)/2)/3.281</f>
         <v>1.1048460835111247</v>
       </c>
-      <c r="F189" s="199"/>
-      <c r="G189" s="214">
+      <c r="F189" s="162"/>
+      <c r="G189" s="177">
         <f t="shared" si="29"/>
         <v>7.733922584577873</v>
       </c>
-      <c r="H189" s="200"/>
-      <c r="I189" s="200"/>
-      <c r="J189" s="200"/>
-      <c r="K189" s="186"/>
-    </row>
-    <row r="190" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A190" s="181"/>
-      <c r="B190" s="183"/>
-      <c r="C190" s="198">
+      <c r="H189" s="163"/>
+      <c r="I189" s="163"/>
+      <c r="J189" s="163"/>
+      <c r="K189" s="149"/>
+    </row>
+    <row r="190" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A190" s="144"/>
+      <c r="B190" s="146"/>
+      <c r="C190" s="161">
         <v>1</v>
       </c>
-      <c r="D190" s="199">
+      <c r="D190" s="162">
         <v>6.55</v>
       </c>
-      <c r="E190" s="199">
+      <c r="E190" s="162">
         <f>((16.17+1)/2)/3.281</f>
         <v>2.616580310880829</v>
       </c>
-      <c r="F190" s="199"/>
-      <c r="G190" s="214">
+      <c r="F190" s="162"/>
+      <c r="G190" s="177">
         <f t="shared" si="29"/>
         <v>17.138601036269428</v>
       </c>
-      <c r="H190" s="200"/>
-      <c r="I190" s="200"/>
-      <c r="J190" s="200"/>
-      <c r="K190" s="186"/>
-    </row>
-    <row r="191" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A191" s="200"/>
-      <c r="B191" s="183" t="s">
+      <c r="H190" s="163"/>
+      <c r="I190" s="163"/>
+      <c r="J190" s="163"/>
+      <c r="K190" s="149"/>
+    </row>
+    <row r="191" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A191" s="163"/>
+      <c r="B191" s="146" t="s">
         <v>41</v>
       </c>
-      <c r="C191" s="205"/>
-      <c r="D191" s="206"/>
-      <c r="E191" s="206"/>
-      <c r="F191" s="206"/>
-      <c r="G191" s="216">
+      <c r="C191" s="168"/>
+      <c r="D191" s="169"/>
+      <c r="E191" s="169"/>
+      <c r="F191" s="169"/>
+      <c r="G191" s="179">
         <f>0*SUM(G186:G190)</f>
         <v>0</v>
       </c>
-      <c r="H191" s="216" t="s">
+      <c r="H191" s="179" t="s">
         <v>141</v>
       </c>
-      <c r="I191" s="216">
+      <c r="I191" s="179">
         <f>35*10.7639</f>
         <v>376.73649999999998</v>
       </c>
-      <c r="J191" s="208">
+      <c r="J191" s="171">
         <f>G191*I191</f>
         <v>0</v>
       </c>
-      <c r="K191" s="198"/>
-    </row>
-    <row r="192" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A192" s="200"/>
-      <c r="B192" s="183" t="s">
+      <c r="K191" s="161"/>
+    </row>
+    <row r="192" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A192" s="163"/>
+      <c r="B192" s="146" t="s">
         <v>40</v>
       </c>
-      <c r="C192" s="205"/>
-      <c r="D192" s="206"/>
-      <c r="E192" s="206"/>
-      <c r="F192" s="206"/>
-      <c r="G192" s="206"/>
-      <c r="H192" s="206"/>
-      <c r="I192" s="206"/>
-      <c r="J192" s="202">
+      <c r="C192" s="168"/>
+      <c r="D192" s="169"/>
+      <c r="E192" s="169"/>
+      <c r="F192" s="169"/>
+      <c r="G192" s="169"/>
+      <c r="H192" s="169"/>
+      <c r="I192" s="169"/>
+      <c r="J192" s="165">
         <f>0.13*J191</f>
         <v>0</v>
       </c>
-      <c r="K192" s="198"/>
-    </row>
-    <row r="193" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A193" s="200"/>
-      <c r="B193" s="183"/>
-      <c r="C193" s="205"/>
-      <c r="D193" s="206"/>
-      <c r="E193" s="206"/>
-      <c r="F193" s="206"/>
-      <c r="G193" s="206"/>
-      <c r="H193" s="206"/>
-      <c r="I193" s="206"/>
-      <c r="J193" s="202"/>
-      <c r="K193" s="198"/>
-    </row>
-    <row r="194" spans="1:22" s="211" customFormat="1" ht="41.4">
-      <c r="A194" s="181">
+      <c r="K192" s="161"/>
+    </row>
+    <row r="193" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A193" s="163"/>
+      <c r="B193" s="146"/>
+      <c r="C193" s="168"/>
+      <c r="D193" s="169"/>
+      <c r="E193" s="169"/>
+      <c r="F193" s="169"/>
+      <c r="G193" s="169"/>
+      <c r="H193" s="169"/>
+      <c r="I193" s="169"/>
+      <c r="J193" s="165"/>
+      <c r="K193" s="161"/>
+    </row>
+    <row r="194" spans="1:22" s="174" customFormat="1" ht="42.75">
+      <c r="A194" s="144">
         <v>19</v>
       </c>
-      <c r="B194" s="217" t="s">
+      <c r="B194" s="180" t="s">
         <v>145</v>
       </c>
-      <c r="C194" s="198"/>
-      <c r="D194" s="199"/>
-      <c r="E194" s="199"/>
-      <c r="F194" s="199"/>
-      <c r="G194" s="187"/>
-      <c r="H194" s="200"/>
-      <c r="I194" s="200"/>
-      <c r="J194" s="202"/>
-      <c r="K194" s="186"/>
-      <c r="M194" s="218"/>
-      <c r="N194" s="218"/>
-      <c r="O194" s="218"/>
-      <c r="P194" s="218"/>
-      <c r="Q194" s="218"/>
-      <c r="R194" s="218"/>
-      <c r="S194" s="218"/>
-      <c r="T194" s="218"/>
-      <c r="U194" s="218"/>
-      <c r="V194" s="218"/>
-    </row>
-    <row r="195" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A195" s="200"/>
-      <c r="B195" s="183" t="s">
+      <c r="C194" s="161"/>
+      <c r="D194" s="162"/>
+      <c r="E194" s="162"/>
+      <c r="F194" s="162"/>
+      <c r="G194" s="150"/>
+      <c r="H194" s="163"/>
+      <c r="I194" s="163"/>
+      <c r="J194" s="165"/>
+      <c r="K194" s="149"/>
+      <c r="M194" s="181"/>
+      <c r="N194" s="181"/>
+      <c r="O194" s="181"/>
+      <c r="P194" s="181"/>
+      <c r="Q194" s="181"/>
+      <c r="R194" s="181"/>
+      <c r="S194" s="181"/>
+      <c r="T194" s="181"/>
+      <c r="U194" s="181"/>
+      <c r="V194" s="181"/>
+    </row>
+    <row r="195" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A195" s="163"/>
+      <c r="B195" s="146" t="s">
         <v>146</v>
       </c>
-      <c r="C195" s="184"/>
-      <c r="D195" s="206"/>
-      <c r="E195" s="206"/>
-      <c r="F195" s="206"/>
-      <c r="G195" s="206">
+      <c r="C195" s="147"/>
+      <c r="D195" s="169"/>
+      <c r="E195" s="169"/>
+      <c r="F195" s="169"/>
+      <c r="G195" s="169">
         <f>G191</f>
         <v>0</v>
       </c>
-      <c r="H195" s="206"/>
-      <c r="I195" s="206"/>
-      <c r="J195" s="202"/>
-      <c r="K195" s="198"/>
-      <c r="M195" s="218"/>
-      <c r="N195" s="218"/>
-      <c r="O195" s="218"/>
-      <c r="P195" s="218"/>
-      <c r="Q195" s="218"/>
-      <c r="R195" s="218"/>
-      <c r="S195" s="218"/>
-      <c r="T195" s="218"/>
-      <c r="U195" s="218"/>
-      <c r="V195" s="218"/>
-    </row>
-    <row r="196" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A196" s="200"/>
-      <c r="B196" s="183" t="str">
+      <c r="H195" s="169"/>
+      <c r="I195" s="169"/>
+      <c r="J195" s="165"/>
+      <c r="K195" s="161"/>
+      <c r="M195" s="181"/>
+      <c r="N195" s="181"/>
+      <c r="O195" s="181"/>
+      <c r="P195" s="181"/>
+      <c r="Q195" s="181"/>
+      <c r="R195" s="181"/>
+      <c r="S195" s="181"/>
+      <c r="T195" s="181"/>
+      <c r="U195" s="181"/>
+      <c r="V195" s="181"/>
+    </row>
+    <row r="196" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A196" s="163"/>
+      <c r="B196" s="146" t="str">
         <f>B117</f>
         <v>-at entrance</v>
       </c>
-      <c r="C196" s="184">
+      <c r="C196" s="147">
         <v>1</v>
       </c>
-      <c r="D196" s="188">
+      <c r="D196" s="151">
         <f>D117</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="E196" s="188">
+      <c r="E196" s="151">
         <f>E117</f>
         <v>0.9</v>
       </c>
-      <c r="F196" s="188"/>
-      <c r="G196" s="214">
+      <c r="F196" s="151"/>
+      <c r="G196" s="177">
         <f t="shared" ref="G196" si="30">PRODUCT(C196:F196)</f>
         <v>1.9800000000000002</v>
       </c>
-      <c r="H196" s="206"/>
-      <c r="I196" s="206"/>
-      <c r="J196" s="202"/>
-      <c r="K196" s="198"/>
-      <c r="M196" s="218"/>
-      <c r="N196" s="218"/>
-      <c r="O196" s="218"/>
-      <c r="P196" s="218"/>
-      <c r="Q196" s="218"/>
-      <c r="R196" s="218"/>
-      <c r="S196" s="218"/>
-      <c r="T196" s="218"/>
-      <c r="U196" s="218"/>
-      <c r="V196" s="218"/>
-    </row>
-    <row r="197" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A197" s="200"/>
-      <c r="B197" s="183" t="s">
+      <c r="H196" s="169"/>
+      <c r="I196" s="169"/>
+      <c r="J196" s="165"/>
+      <c r="K196" s="161"/>
+      <c r="M196" s="181"/>
+      <c r="N196" s="181"/>
+      <c r="O196" s="181"/>
+      <c r="P196" s="181"/>
+      <c r="Q196" s="181"/>
+      <c r="R196" s="181"/>
+      <c r="S196" s="181"/>
+      <c r="T196" s="181"/>
+      <c r="U196" s="181"/>
+      <c r="V196" s="181"/>
+    </row>
+    <row r="197" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A197" s="163"/>
+      <c r="B197" s="146" t="s">
         <v>41</v>
       </c>
-      <c r="C197" s="205"/>
-      <c r="D197" s="206"/>
-      <c r="E197" s="206"/>
-      <c r="F197" s="206"/>
-      <c r="G197" s="216">
+      <c r="C197" s="168"/>
+      <c r="D197" s="169"/>
+      <c r="E197" s="169"/>
+      <c r="F197" s="169"/>
+      <c r="G197" s="179">
         <f>0*SUM(G195:G196)</f>
         <v>0</v>
       </c>
-      <c r="H197" s="216" t="s">
+      <c r="H197" s="179" t="s">
         <v>141</v>
       </c>
-      <c r="I197" s="216">
+      <c r="I197" s="179">
         <v>9.1999999999999993</v>
       </c>
-      <c r="J197" s="208">
+      <c r="J197" s="171">
         <f>G197*I197</f>
         <v>0</v>
       </c>
-      <c r="K197" s="198"/>
-      <c r="M197" s="218"/>
-      <c r="N197" s="218"/>
-      <c r="O197" s="218"/>
-      <c r="P197" s="218"/>
-      <c r="Q197" s="218"/>
-      <c r="R197" s="218"/>
-      <c r="S197" s="218"/>
-      <c r="T197" s="218"/>
-      <c r="U197" s="218"/>
-      <c r="V197" s="218"/>
-    </row>
-    <row r="198" spans="1:22" s="211" customFormat="1" ht="15" customHeight="1">
-      <c r="A198" s="181"/>
-      <c r="B198" s="183"/>
-      <c r="C198" s="184"/>
-      <c r="D198" s="185"/>
-      <c r="E198" s="186"/>
-      <c r="F198" s="186"/>
-      <c r="G198" s="195"/>
-      <c r="H198" s="196"/>
-      <c r="I198" s="195"/>
-      <c r="J198" s="197"/>
-      <c r="K198" s="186"/>
-      <c r="M198" s="218"/>
-      <c r="N198" s="218"/>
-      <c r="O198" s="218"/>
-      <c r="P198" s="218"/>
-      <c r="Q198" s="218"/>
-      <c r="R198" s="218"/>
-      <c r="S198" s="218"/>
-      <c r="T198" s="218"/>
-      <c r="U198" s="218"/>
-      <c r="V198" s="218"/>
+      <c r="K197" s="161"/>
+      <c r="M197" s="181"/>
+      <c r="N197" s="181"/>
+      <c r="O197" s="181"/>
+      <c r="P197" s="181"/>
+      <c r="Q197" s="181"/>
+      <c r="R197" s="181"/>
+      <c r="S197" s="181"/>
+      <c r="T197" s="181"/>
+      <c r="U197" s="181"/>
+      <c r="V197" s="181"/>
+    </row>
+    <row r="198" spans="1:22" s="174" customFormat="1" ht="15" customHeight="1">
+      <c r="A198" s="144"/>
+      <c r="B198" s="146"/>
+      <c r="C198" s="147"/>
+      <c r="D198" s="148"/>
+      <c r="E198" s="149"/>
+      <c r="F198" s="149"/>
+      <c r="G198" s="158"/>
+      <c r="H198" s="159"/>
+      <c r="I198" s="158"/>
+      <c r="J198" s="160"/>
+      <c r="K198" s="149"/>
+      <c r="M198" s="181"/>
+      <c r="N198" s="181"/>
+      <c r="O198" s="181"/>
+      <c r="P198" s="181"/>
+      <c r="Q198" s="181"/>
+      <c r="R198" s="181"/>
+      <c r="S198" s="181"/>
+      <c r="T198" s="181"/>
+      <c r="U198" s="181"/>
+      <c r="V198" s="181"/>
     </row>
     <row r="199" spans="1:22" ht="15" customHeight="1">
       <c r="A199" s="18">
@@ -13921,7 +13932,7 @@
       <c r="I203" s="39"/>
       <c r="J203" s="39">
         <f>SUM(J10:J201)</f>
-        <v>450558.50226700824</v>
+        <v>425480.08486204845</v>
       </c>
       <c r="K203" s="34"/>
       <c r="M203" s="33"/>
@@ -13961,13 +13972,13 @@
     <row r="205" spans="1:22" s="1" customFormat="1">
       <c r="A205" s="45"/>
       <c r="B205" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C205" s="164">
+        <v>166</v>
+      </c>
+      <c r="C205" s="185">
         <f>J203</f>
-        <v>450558.50226700824</v>
-      </c>
-      <c r="D205" s="164"/>
+        <v>425480.08486204845</v>
+      </c>
+      <c r="D205" s="185"/>
       <c r="E205" s="37">
         <v>100</v>
       </c>
@@ -13993,10 +14004,10 @@
       <c r="B206" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C206" s="165">
+      <c r="C206" s="187">
         <v>500000</v>
       </c>
-      <c r="D206" s="165"/>
+      <c r="D206" s="187"/>
       <c r="E206" s="37"/>
       <c r="F206" s="44"/>
       <c r="G206" s="43"/>
@@ -14020,14 +14031,14 @@
       <c r="B207" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C207" s="165">
+      <c r="C207" s="187">
         <f>C206-C209-C210</f>
         <v>475000</v>
       </c>
-      <c r="D207" s="165"/>
+      <c r="D207" s="187"/>
       <c r="E207" s="37">
         <f>C207/C205*100</f>
-        <v>105.42471124393683</v>
+        <v>111.63859764529454</v>
       </c>
       <c r="F207" s="44"/>
       <c r="G207" s="43"/>
@@ -14051,14 +14062,14 @@
       <c r="B208" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C208" s="164">
+      <c r="C208" s="185">
         <f>C205-C207</f>
-        <v>-24441.49773299176</v>
-      </c>
-      <c r="D208" s="164"/>
+        <v>-49519.915137951553</v>
+      </c>
+      <c r="D208" s="185"/>
       <c r="E208" s="37">
         <f>100-E207</f>
-        <v>-5.4247112439368266</v>
+        <v>-11.638597645294539</v>
       </c>
       <c r="F208" s="44"/>
       <c r="G208" s="43"/>
@@ -14082,11 +14093,11 @@
       <c r="B209" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C209" s="164">
+      <c r="C209" s="185">
         <f>C206*0.03</f>
         <v>15000</v>
       </c>
-      <c r="D209" s="164"/>
+      <c r="D209" s="185"/>
       <c r="E209" s="37">
         <v>3</v>
       </c>
@@ -14112,11 +14123,11 @@
       <c r="B210" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C210" s="164">
+      <c r="C210" s="185">
         <f>C206*0.02</f>
         <v>10000</v>
       </c>
-      <c r="D210" s="164"/>
+      <c r="D210" s="185"/>
       <c r="E210" s="37">
         <v>2</v>
       </c>
@@ -14395,13 +14406,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C210:D210"/>
-    <mergeCell ref="N172:T172"/>
-    <mergeCell ref="C205:D205"/>
-    <mergeCell ref="C206:D206"/>
-    <mergeCell ref="C207:D207"/>
-    <mergeCell ref="C208:D208"/>
-    <mergeCell ref="C209:D209"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="N83:T83"/>
@@ -14413,6 +14417,13 @@
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
+    <mergeCell ref="C210:D210"/>
+    <mergeCell ref="N172:T172"/>
+    <mergeCell ref="C205:D205"/>
+    <mergeCell ref="C206:D206"/>
+    <mergeCell ref="C207:D207"/>
+    <mergeCell ref="C208:D208"/>
+    <mergeCell ref="C209:D209"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B140" r:id="rId1"/>

</xml_diff>